<commit_message>
update the deming parameters
</commit_message>
<xml_diff>
--- a/deming.xlsx
+++ b/deming.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C281"/>
+  <dimension ref="A1:C283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,3546 +453,3550 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>298</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.0193</v>
+        <v>0.0018</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0969</v>
+        <v>0.3676</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>297</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.014</v>
+        <v>-0.0302</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0963</v>
+        <v>0.6565</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>296</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.0133</v>
+        <v>-0.0643</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5499000000000001</v>
+        <v>0.6147</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>295</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.0007</v>
+        <v>-0.0163</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1461</v>
+        <v>0.0958</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>293</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.022</v>
+        <v>-0.0191</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1821</v>
+        <v>0.1281</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>292</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0573</v>
+        <v>-0.0002</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3502</v>
+        <v>0.1981</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>291</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.0287</v>
+        <v>0.0015</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1993</v>
+        <v>0.3166</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>290</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-0.0038</v>
       </c>
       <c r="C9" t="n">
-        <v>1.25</v>
+        <v>0.742</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>288</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.034</v>
+        <v>0.0179</v>
       </c>
       <c r="C10" t="n">
-        <v>0.668</v>
+        <v>0.4822</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>287</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.287</v>
+        <v>0.0316</v>
       </c>
       <c r="C11" t="n">
-        <v>0.321</v>
+        <v>0.6574</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>284</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.0173</v>
+        <v>-0.0112</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4164</v>
+        <v>0.1015</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>281</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.14</v>
+        <v>0.0186</v>
       </c>
       <c r="C13" t="n">
-        <v>0.704</v>
+        <v>0.1738</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>280</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.106</v>
+        <v>-0.0844</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6702</v>
+        <v>0.1891</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>279</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.016</v>
+        <v>0.0557</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3869</v>
+        <v>0.2566</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>278</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.0147</v>
+        <v>0.0015</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1721</v>
+        <v>0.3175</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>276</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0007</v>
+        <v>0.0031</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1467</v>
+        <v>0.1311</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>275</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.018</v>
+        <v>0.08309999999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2039</v>
+        <v>0.1619</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>274</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.1773</v>
+        <v>-0.0156</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3019</v>
+        <v>0.2041</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>271</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.0707</v>
+        <v>0.0515</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3155</v>
+        <v>0.1889</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>267</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.009299999999999999</v>
+        <v>0.0025</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0815</v>
+        <v>0.2421</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>266</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.0033</v>
+        <v>-0.0304</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2852</v>
+        <v>0.4378</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>264</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.0053</v>
+        <v>-0.0044</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2126</v>
+        <v>0.2959</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>263</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.012</v>
+        <v>0.0709</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2106</v>
+        <v>0.2036</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>262</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.0073</v>
+        <v>0.0131</v>
       </c>
       <c r="C25" t="n">
-        <v>0.214</v>
+        <v>0.1006</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>261</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.035</v>
+        <v>0.1376</v>
       </c>
       <c r="C26" t="n">
-        <v>0.4043</v>
+        <v>0.3925</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>260</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.0027</v>
+        <v>-0.0116</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5021</v>
+        <v>0.3037</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>258</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.0007</v>
+        <v>-0.0415</v>
       </c>
       <c r="C28" t="n">
-        <v>0.212</v>
+        <v>0.5963000000000001</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>257</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.006</v>
+        <v>-0.0157</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1417</v>
+        <v>0.4804</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>256</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.01</v>
+        <v>-0.0242</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1028</v>
+        <v>0.1822</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>255</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.03</v>
+        <v>0.027</v>
       </c>
       <c r="C31" t="n">
-        <v>0.3637</v>
+        <v>0.1701</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>254</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.0147</v>
+        <v>0.2372</v>
       </c>
       <c r="C32" t="n">
-        <v>0.2581</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>253</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.0153</v>
+        <v>0.0616</v>
       </c>
       <c r="C33" t="n">
-        <v>1.6582</v>
+        <v>0.2351</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>252</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.0107</v>
+        <v>0.0852</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1216</v>
+        <v>0.2099</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>251</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.004</v>
+        <v>0.0238</v>
       </c>
       <c r="C35" t="n">
-        <v>0.2023</v>
+        <v>0.2664</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.0007</v>
+        <v>0.07190000000000001</v>
       </c>
       <c r="C36" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.1947</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-0.018</v>
+        <v>0.0322</v>
       </c>
       <c r="C37" t="n">
-        <v>0.4303</v>
+        <v>0.3508</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.0113</v>
+        <v>-0.0208</v>
       </c>
       <c r="C38" t="n">
-        <v>0.3976</v>
+        <v>0.1824</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.0033</v>
+        <v>-0.0372</v>
       </c>
       <c r="C39" t="n">
-        <v>0.132</v>
+        <v>0.4311</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-0.01</v>
+        <v>-0.0228</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1767</v>
+        <v>0.0863</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-0.028</v>
+        <v>0.0312</v>
       </c>
       <c r="C41" t="n">
-        <v>0.309</v>
+        <v>0.2015</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.008699999999999999</v>
+        <v>-0.0612</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1557</v>
+        <v>0.1231</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-0.0013</v>
+        <v>0.0935</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1242</v>
+        <v>1.6582</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-0.002</v>
+        <v>-0.0052</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1294</v>
+        <v>0.2578</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-0.002</v>
+        <v>0.0343</v>
       </c>
       <c r="C45" t="n">
-        <v>0.2031</v>
+        <v>0.3642</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>40</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0295</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1922</v>
+        <v>0.1025</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.006</v>
+        <v>-0.0237</v>
       </c>
       <c r="C47" t="n">
-        <v>0.4718</v>
+        <v>0.1463</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-0.0033</v>
+        <v>0.0556</v>
       </c>
       <c r="C48" t="n">
-        <v>0.3355</v>
+        <v>0.1401</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>38</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.0273</v>
+        <v>-0.0055</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2064</v>
+        <v>0.2114</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-0.0273</v>
+        <v>-0.0091</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1015</v>
+        <v>0.5024</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.0133</v>
+        <v>0.0016</v>
       </c>
       <c r="C51" t="n">
-        <v>0.281</v>
+        <v>0.4061</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0819</v>
       </c>
       <c r="C52" t="n">
-        <v>0.1927</v>
+        <v>0.2125</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-0.0107</v>
+        <v>0.0132</v>
       </c>
       <c r="C53" t="n">
-        <v>0.2105</v>
+        <v>0.2106</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-0.0273</v>
+        <v>0.0335</v>
       </c>
       <c r="C54" t="n">
-        <v>0.09760000000000001</v>
+        <v>0.2124</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.0213</v>
+        <v>-0.1532</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1023</v>
+        <v>0.5537</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-0.005</v>
+        <v>-0.0161</v>
       </c>
       <c r="C56" t="n">
-        <v>0.1027</v>
+        <v>0.2852</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>-0.008</v>
+        <v>0.0312</v>
       </c>
       <c r="C57" t="n">
-        <v>0.4213</v>
+        <v>0.08119999999999999</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.0759</v>
+        <v>0.0219</v>
       </c>
       <c r="C58" t="n">
-        <v>0.5598</v>
+        <v>0.3161</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.0233</v>
+        <v>0.1666</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0756</v>
+        <v>0.3027</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-0.014</v>
+        <v>0.07729999999999999</v>
       </c>
       <c r="C60" t="n">
-        <v>0.2255</v>
+        <v>0.145</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-0.0047</v>
+        <v>0.0263</v>
       </c>
       <c r="C61" t="n">
-        <v>0.1136</v>
+        <v>0.0951</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.038</v>
+        <v>0.0707</v>
       </c>
       <c r="C62" t="n">
-        <v>0.8113</v>
+        <v>0.1699</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-0.018</v>
+        <v>0.022</v>
       </c>
       <c r="C63" t="n">
-        <v>0.08790000000000001</v>
+        <v>0.3866</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-0.0147</v>
+        <v>0.1082</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1738</v>
+        <v>0.6686</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-0.008</v>
+        <v>0.039</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3827</v>
+        <v>0.6963</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-0.0053</v>
+        <v>0.07140000000000001</v>
       </c>
       <c r="C66" t="n">
-        <v>0.1035</v>
+        <v>0.4161</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>-0.032</v>
+        <v>0.4584</v>
       </c>
       <c r="C67" t="n">
-        <v>0.3539</v>
+        <v>0.3191</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>-0.004</v>
+        <v>-0.349</v>
       </c>
       <c r="C68" t="n">
-        <v>0.2067</v>
+        <v>0.6813</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.0467</v>
+        <v>-0.1548</v>
       </c>
       <c r="C69" t="n">
-        <v>0.6322</v>
+        <v>1.2659</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>-0.0153</v>
+        <v>0.0023</v>
       </c>
       <c r="C70" t="n">
-        <v>0.1564</v>
+        <v>0.0964</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>350</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.0953</v>
+        <v>0.0718</v>
       </c>
       <c r="C71" t="n">
-        <v>0.6299</v>
+        <v>1.023</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>-0.006</v>
+        <v>0.0008</v>
       </c>
       <c r="C72" t="n">
-        <v>0.3712</v>
+        <v>0.1673</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>347</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-0.0157</v>
+        <v>0.0229</v>
       </c>
       <c r="C73" t="n">
-        <v>0.128</v>
+        <v>0.3054</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>346</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-0.004</v>
+        <v>0.0023</v>
       </c>
       <c r="C74" t="n">
-        <v>0.4104</v>
+        <v>0.07489999999999999</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>345</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-0.0393</v>
+        <v>0.0827</v>
       </c>
       <c r="C75" t="n">
-        <v>0.7486</v>
+        <v>0.1248</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>343</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>-0.0247</v>
+        <v>-0.184</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7000999999999999</v>
+        <v>0.296</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.0107</v>
+        <v>0.0843</v>
       </c>
       <c r="C77" t="n">
-        <v>0.3862</v>
+        <v>0.2048</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>341</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-0.0227</v>
+        <v>0.0591</v>
       </c>
       <c r="C78" t="n">
-        <v>0.066</v>
+        <v>0.2658</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.0067</v>
+        <v>0.2156</v>
       </c>
       <c r="C79" t="n">
-        <v>0.2951</v>
+        <v>0.5736</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>338</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>-0.0207</v>
+        <v>-0.08599999999999999</v>
       </c>
       <c r="C80" t="n">
-        <v>0.3238</v>
+        <v>0.6538</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>337</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.0327</v>
+        <v>-0.0892</v>
       </c>
       <c r="C81" t="n">
-        <v>0.2364</v>
+        <v>0.5678</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>335</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.0073</v>
+        <v>-0.0172</v>
       </c>
       <c r="C82" t="n">
-        <v>0.3539</v>
+        <v>0.2505</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>334</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.0033</v>
+        <v>-0.0036</v>
       </c>
       <c r="C83" t="n">
-        <v>0.4806</v>
+        <v>0.2124</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>333</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-0.008699999999999999</v>
+        <v>0.0046</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1248</v>
+        <v>0.4445</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>332</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.01</v>
+        <v>0.0574</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1209</v>
+        <v>0.1032</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>331</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>-0.01</v>
+        <v>0.0321</v>
       </c>
       <c r="C86" t="n">
-        <v>0.1812</v>
+        <v>0.4845</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>330</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.0053</v>
+        <v>0.0131</v>
       </c>
       <c r="C87" t="n">
-        <v>0.3349</v>
+        <v>0.2559</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>329</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.064</v>
+        <v>0.0326</v>
       </c>
       <c r="C88" t="n">
-        <v>0.2025</v>
+        <v>0.162</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>328</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-0.0193</v>
+        <v>0.0243</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1216</v>
+        <v>0.2076</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>326</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-0</v>
+        <v>-0.014</v>
       </c>
       <c r="C90" t="n">
-        <v>0.2975</v>
+        <v>0.0502</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>325</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-0.0193</v>
+        <v>0.1078</v>
       </c>
       <c r="C91" t="n">
-        <v>0.1532</v>
+        <v>0.2098</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>324</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.038</v>
+        <v>0.043</v>
       </c>
       <c r="C92" t="n">
-        <v>0.181</v>
+        <v>0.3091</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>323</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-0.0267</v>
+        <v>0.0165</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1089</v>
+        <v>0.1048</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>320</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.0007</v>
+        <v>0.017</v>
       </c>
       <c r="C94" t="n">
-        <v>0.07539999999999999</v>
+        <v>0.2305</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>319</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-0.0053</v>
+        <v>-0.0162</v>
       </c>
       <c r="C95" t="n">
-        <v>0.2114</v>
+        <v>0.1248</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>317</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-0.0073</v>
+        <v>0.0746</v>
       </c>
       <c r="C96" t="n">
-        <v>0.1722</v>
+        <v>0.5271</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>316</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.1066</v>
+        <v>-0.08110000000000001</v>
       </c>
       <c r="C97" t="n">
-        <v>0.325</v>
+        <v>0.6222</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>315</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-0.0053</v>
+        <v>-0.07340000000000001</v>
       </c>
       <c r="C98" t="n">
-        <v>0.184</v>
+        <v>0.6687</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>314</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>-0.028</v>
+        <v>-0.0257</v>
       </c>
       <c r="C99" t="n">
-        <v>0.2126</v>
+        <v>0.3176</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>313</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.004</v>
+        <v>-0.0505</v>
       </c>
       <c r="C100" t="n">
-        <v>0.1022</v>
+        <v>0.1028</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>312</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.02</v>
+        <v>0.0003</v>
       </c>
       <c r="C101" t="n">
-        <v>0.4031</v>
+        <v>0.2077</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>308</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.002</v>
+        <v>0.0013</v>
       </c>
       <c r="C102" t="n">
-        <v>0.1049</v>
+        <v>0.543</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>-0</v>
+        <v>0.1328</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1255</v>
+        <v>0.2289</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>-0.0347</v>
+        <v>0.0168</v>
       </c>
       <c r="C104" t="n">
-        <v>0.281</v>
+        <v>0.1262</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.008699999999999999</v>
+        <v>-0.005</v>
       </c>
       <c r="C105" t="n">
-        <v>0.25</v>
+        <v>0.0974</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>304</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-0.0207</v>
+        <v>-0.0273</v>
       </c>
       <c r="C106" t="n">
-        <v>0.1748</v>
+        <v>0.0964</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>303</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.0013</v>
+        <v>-0.0144</v>
       </c>
       <c r="C107" t="n">
-        <v>0.1017</v>
+        <v>0.142</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>152</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr"/>
-      <c r="C108" t="inlineStr"/>
+          <t>302</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>0.0236</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0.1607</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>98</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-0.032</v>
+        <v>-0.0134</v>
       </c>
       <c r="C109" t="n">
-        <v>0.5383</v>
+        <v>0.1563</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>97</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.002</v>
+        <v>0.0622</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1549</v>
+        <v>0.6319</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>96</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-0.0173</v>
+        <v>-0.0101</v>
       </c>
       <c r="C111" t="n">
-        <v>0.1727</v>
+        <v>0.2069</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>95</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.0047</v>
+        <v>-0.0298</v>
       </c>
       <c r="C112" t="n">
-        <v>0.1738</v>
+        <v>0.354</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>92</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.0227</v>
+        <v>0.009599999999999999</v>
       </c>
       <c r="C113" t="n">
-        <v>0.2112</v>
+        <v>0.103</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>158</t>
+          <t>91</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.008699999999999999</v>
+        <v>-0.1687</v>
       </c>
       <c r="C114" t="n">
-        <v>0.2017</v>
+        <v>0.387</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>90</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-0.0027</v>
+        <v>-0.0593</v>
       </c>
       <c r="C115" t="n">
-        <v>0.09619999999999999</v>
+        <v>0.1746</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>161</t>
+          <t>89</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.0433</v>
+        <v>-0.0218</v>
       </c>
       <c r="C116" t="n">
-        <v>0.2619</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>87</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.004</v>
+        <v>0.0142</v>
       </c>
       <c r="C117" t="n">
-        <v>0.5503</v>
+        <v>0.8121</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>164</t>
+          <t>83</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.0013</v>
+        <v>0.0169</v>
       </c>
       <c r="C118" t="n">
-        <v>0.1633</v>
+        <v>0.1131</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>82</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-0.004</v>
+        <v>0.0519</v>
       </c>
       <c r="C119" t="n">
-        <v>0.2499</v>
+        <v>0.2238</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>81</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.094</v>
+        <v>-0.0116</v>
       </c>
       <c r="C120" t="n">
-        <v>0.4137</v>
+        <v>0.0756</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>80</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.0053</v>
+        <v>0.29</v>
       </c>
       <c r="C121" t="n">
-        <v>0.4874</v>
+        <v>0.5531</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>79</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0.0193</v>
+        <v>-0.0112</v>
       </c>
       <c r="C122" t="n">
-        <v>0.2798</v>
+        <v>0.4234</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>171</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.0033</v>
+        <v>0.0774</v>
       </c>
       <c r="C123" t="n">
-        <v>0.2019</v>
+        <v>0.0999</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>75</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.0173</v>
+        <v>-0.0238</v>
       </c>
       <c r="C124" t="n">
-        <v>0.5341</v>
+        <v>0.1022</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>74</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.0307</v>
+        <v>0.0105</v>
       </c>
       <c r="C125" t="n">
-        <v>0.4106</v>
+        <v>0.097</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.0213</v>
+        <v>-0.0303</v>
       </c>
       <c r="C126" t="n">
-        <v>0.1033</v>
+        <v>0.2122</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>71</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.0886</v>
+        <v>-0.0071</v>
       </c>
       <c r="C127" t="n">
-        <v>0.2668</v>
+        <v>0.1928</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>179</t>
+          <t>70</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0</v>
+        <v>-0.0005999999999999999</v>
       </c>
       <c r="C128" t="n">
-        <v>0.2399</v>
+        <v>0.281</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>69</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-0.0013</v>
+        <v>-0.0116</v>
       </c>
       <c r="C129" t="n">
-        <v>0.1718</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>67</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-0.032</v>
+        <v>0.0799</v>
       </c>
       <c r="C130" t="n">
-        <v>0.4194</v>
+        <v>0.2055</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>183</t>
+          <t>66</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>-0.0287</v>
+        <v>0.1967</v>
       </c>
       <c r="C131" t="n">
-        <v>0.2614</v>
+        <v>0.3307</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.1318</v>
+        <v>0.2237</v>
       </c>
       <c r="C132" t="n">
-        <v>0.7102000000000001</v>
+        <v>0.4687</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>188</t>
+          <t>64</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.0353</v>
+        <v>0.0245</v>
       </c>
       <c r="C133" t="n">
-        <v>0.3128</v>
+        <v>0.1917</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>63</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.08459999999999999</v>
+        <v>-0.0304</v>
       </c>
       <c r="C134" t="n">
-        <v>1.0259</v>
+        <v>0.204</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>62</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>-0.0053</v>
+        <v>-0.016</v>
       </c>
       <c r="C135" t="n">
-        <v>0.211</v>
+        <v>0.1313</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.032</v>
+        <v>-0.0202</v>
       </c>
       <c r="C136" t="n">
-        <v>0.285</v>
+        <v>0.1259</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>-0.0193</v>
+        <v>-0.0022</v>
       </c>
       <c r="C137" t="n">
-        <v>0.5634</v>
+        <v>0.1559</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>196</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.008699999999999999</v>
+        <v>-0.0159</v>
       </c>
       <c r="C138" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.3088</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>-0.038</v>
+        <v>0.0043</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1627</v>
+        <v>0.1766</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>202</t>
+          <t>52</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>-0.0207</v>
+        <v>0.1254</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1661</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>51</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.0213</v>
+        <v>0.106</v>
       </c>
       <c r="C141" t="n">
-        <v>0.2094</v>
+        <v>0.397</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>100</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>-0.0293</v>
+        <v>-0.5258</v>
       </c>
       <c r="C142" t="n">
-        <v>0.1112</v>
+        <v>0.6429</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>149</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.0007</v>
+        <v>0.0041</v>
       </c>
       <c r="C143" t="n">
-        <v>0.2157</v>
+        <v>0.1015</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>148</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-0.0153</v>
+        <v>0.0455</v>
       </c>
       <c r="C144" t="n">
-        <v>0.4232</v>
+        <v>0.1755</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>147</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>-0.1954</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="C145" t="n">
-        <v>0.4928</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>146</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.024</v>
+        <v>-0.0256</v>
       </c>
       <c r="C146" t="n">
-        <v>0.4072</v>
+        <v>0.281</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>145</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.0307</v>
+        <v>0.0421</v>
       </c>
       <c r="C147" t="n">
-        <v>0.188</v>
+        <v>0.1244</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>143</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.012</v>
+        <v>-0.0091</v>
       </c>
       <c r="C148" t="n">
-        <v>0.5795</v>
+        <v>0.1053</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>142</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.0553</v>
+        <v>0.0309</v>
       </c>
       <c r="C149" t="n">
-        <v>0.7167</v>
+        <v>0.4025</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>141</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>-0.0047</v>
+        <v>0.021</v>
       </c>
       <c r="C150" t="n">
-        <v>0.3169</v>
+        <v>0.1019</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>140</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>-0.022</v>
+        <v>-0.0882</v>
       </c>
       <c r="C151" t="n">
-        <v>0.1393</v>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>139</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.0353</v>
+        <v>0.0397</v>
       </c>
       <c r="C152" t="n">
-        <v>0.8229</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>138</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>-0.0333</v>
+        <v>0.0654</v>
       </c>
       <c r="C153" t="n">
-        <v>0.2068</v>
+        <v>0.326</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>137</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.0107</v>
+        <v>-0.0016</v>
       </c>
       <c r="C154" t="n">
-        <v>0.1262</v>
+        <v>0.1722</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>136</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>-0.024</v>
+        <v>-0.0136</v>
       </c>
       <c r="C155" t="n">
-        <v>0.5565</v>
+        <v>0.2111</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>135</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>-0.0127</v>
+        <v>0.0028</v>
       </c>
       <c r="C156" t="n">
-        <v>0.0612</v>
+        <v>0.0764</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>134</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>-0.0207</v>
+        <v>-0.018</v>
       </c>
       <c r="C157" t="n">
-        <v>0.181</v>
+        <v>0.1091</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>-0.0167</v>
+        <v>0.0405</v>
       </c>
       <c r="C158" t="n">
-        <v>0.369</v>
+        <v>0.181</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>226</t>
+          <t>132</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>-0</v>
+        <v>0.053</v>
       </c>
       <c r="C159" t="n">
-        <v>0.1193</v>
+        <v>0.1515</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>228</t>
+          <t>131</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.0247</v>
+        <v>-0.012</v>
       </c>
       <c r="C160" t="n">
-        <v>0.3498</v>
+        <v>0.2976</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>229</t>
+          <t>130</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>-0.0027</v>
+        <v>-0.0181</v>
       </c>
       <c r="C161" t="n">
-        <v>0.1822</v>
+        <v>0.1215</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>129</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.03</v>
+        <v>-0.0335</v>
       </c>
       <c r="C162" t="n">
-        <v>0.4225</v>
+        <v>0.2029</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>128</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.0333</v>
+        <v>0.0014</v>
       </c>
       <c r="C163" t="n">
-        <v>0.4263</v>
+        <v>0.335</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>233</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>-0.006</v>
+        <v>-0.0154</v>
       </c>
       <c r="C164" t="n">
-        <v>0.1199</v>
+        <v>0.2669</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>234</t>
+          <t>124</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>-0.01</v>
+        <v>0.0055</v>
       </c>
       <c r="C165" t="n">
-        <v>0.0741</v>
+        <v>0.1817</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>237</t>
+          <t>122</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>-0.0687</v>
+        <v>-0.0004</v>
       </c>
       <c r="C166" t="n">
-        <v>0.2868</v>
+        <v>0.1213</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>121</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>-0.03</v>
+        <v>-0.3033</v>
       </c>
       <c r="C167" t="n">
-        <v>0.4259</v>
+        <v>0.1308</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>120</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.0387</v>
+        <v>-0.0887</v>
       </c>
       <c r="C168" t="n">
-        <v>0.4058</v>
+        <v>0.4833</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>117</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.0307</v>
+        <v>0.2813</v>
       </c>
       <c r="C169" t="n">
-        <v>0.3668</v>
+        <v>0.3482</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>116</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>-0.0013</v>
+        <v>-0.0106</v>
       </c>
       <c r="C170" t="n">
-        <v>0.3182</v>
+        <v>0.2364</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>115</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.016</v>
+        <v>-0.0675</v>
       </c>
       <c r="C171" t="n">
-        <v>0.2369</v>
+        <v>0.3253</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>114</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.01</v>
+        <v>-0.039</v>
       </c>
       <c r="C172" t="n">
-        <v>0.1407</v>
+        <v>0.2977</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>111</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.0187</v>
+        <v>-0.0144</v>
       </c>
       <c r="C173" t="n">
-        <v>0.1325</v>
+        <v>0.0658</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.0113</v>
+        <v>-0.0313</v>
       </c>
       <c r="C174" t="n">
-        <v>0.2664</v>
+        <v>0.3863</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>107</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.06270000000000001</v>
+        <v>-0.0893</v>
       </c>
       <c r="C175" t="n">
-        <v>0.2098</v>
+        <v>0.7023</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>253</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.0127</v>
+        <v>0.0169</v>
       </c>
       <c r="C176" t="n">
-        <v>0.2364</v>
+        <v>0.7485000000000001</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>104</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.018</v>
+        <v>0.0008</v>
       </c>
       <c r="C177" t="n">
-        <v>0.5538999999999999</v>
+        <v>0.4123</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>103</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.0067</v>
+        <v>-0.008500000000000001</v>
       </c>
       <c r="C178" t="n">
-        <v>0.1706</v>
+        <v>0.1279</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>101</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.004</v>
+        <v>-0.4228</v>
       </c>
       <c r="C179" t="n">
-        <v>0.1815</v>
+        <v>0.3811</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>257</t>
+          <t>383</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>-0.0487</v>
+        <v>-0.08409999999999999</v>
       </c>
       <c r="C180" t="n">
-        <v>0.4809</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>382</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>-0.016</v>
+        <v>0.0934</v>
       </c>
       <c r="C181" t="n">
-        <v>0.5968</v>
+        <v>0.1577</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>260</t>
+          <t>381</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>-0.0193</v>
+        <v>0.092</v>
       </c>
       <c r="C182" t="n">
-        <v>0.3038</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>261</t>
+          <t>380</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>-0.0547</v>
+        <v>0.0241</v>
       </c>
       <c r="C183" t="n">
-        <v>0.3938</v>
+        <v>0.3829</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>263</t>
+          <t>379</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0.0033</v>
+        <v>0.0337</v>
       </c>
       <c r="C184" t="n">
-        <v>0.2052</v>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>264</t>
+          <t>378</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0.014</v>
+        <v>0.0251</v>
       </c>
       <c r="C185" t="n">
-        <v>0.2946</v>
+        <v>0.3386</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>266</t>
+          <t>377</t>
         </is>
       </c>
       <c r="B186" t="n">
-        <v>0.004</v>
+        <v>-0.0052</v>
       </c>
       <c r="C186" t="n">
-        <v>0.4372</v>
+        <v>0.326</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>376</t>
         </is>
       </c>
       <c r="B187" t="n">
-        <v>0.03</v>
+        <v>0.0234</v>
       </c>
       <c r="C187" t="n">
-        <v>0.2421</v>
+        <v>0.1906</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>271</t>
+          <t>374</t>
         </is>
       </c>
       <c r="B188" t="n">
-        <v>-0</v>
+        <v>0.0561</v>
       </c>
       <c r="C188" t="n">
-        <v>0.1887</v>
+        <v>0.2073</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>274</t>
+          <t>373</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>0.0373</v>
+        <v>0.01</v>
       </c>
       <c r="C189" t="n">
-        <v>0.2045</v>
+        <v>0.2381</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>275</t>
+          <t>372</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.0067</v>
+        <v>0.057</v>
       </c>
       <c r="C190" t="n">
-        <v>0.169</v>
+        <v>0.1793</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>276</t>
+          <t>370</t>
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.0033</v>
+        <v>0.0057</v>
       </c>
       <c r="C191" t="n">
-        <v>0.1312</v>
+        <v>0.1562</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>369</t>
         </is>
       </c>
       <c r="B192" t="n">
-        <v>-0.0027</v>
+        <v>0.0102</v>
       </c>
       <c r="C192" t="n">
-        <v>0.3179</v>
+        <v>0.135</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>279</t>
+          <t>367</t>
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.042</v>
+        <v>0.0043</v>
       </c>
       <c r="C193" t="n">
-        <v>0.2567</v>
+        <v>0.215</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>280</t>
+          <t>364</t>
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0.0027</v>
+        <v>-0.0005999999999999999</v>
       </c>
       <c r="C194" t="n">
-        <v>0.1869</v>
+        <v>0.0891</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>281</t>
+          <t>362</t>
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0.0107</v>
+        <v>-0.1235</v>
       </c>
       <c r="C195" t="n">
-        <v>0.1739</v>
+        <v>0.3601</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>361</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>-0.0027</v>
+        <v>0.0111</v>
       </c>
       <c r="C196" t="n">
-        <v>0.1013</v>
+        <v>0.5265</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>287</t>
+          <t>360</t>
         </is>
       </c>
       <c r="B197" t="n">
-        <v>-0.036</v>
+        <v>-0.0333</v>
       </c>
       <c r="C197" t="n">
-        <v>0.659</v>
+        <v>0.2992</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>288</t>
+          <t>359</t>
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.0173</v>
+        <v>-0.058</v>
       </c>
       <c r="C198" t="n">
-        <v>0.4825</v>
+        <v>0.2198</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>354</t>
         </is>
       </c>
       <c r="B199" t="n">
-        <v>-0.008699999999999999</v>
+        <v>-0.0299</v>
       </c>
       <c r="C199" t="n">
-        <v>0.7415</v>
+        <v>0.1044</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>291</t>
+          <t>353</t>
         </is>
       </c>
       <c r="B200" t="n">
-        <v>0.002</v>
+        <v>0.0156</v>
       </c>
       <c r="C200" t="n">
-        <v>0.3166</v>
+        <v>0.4178</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>292</t>
+          <t>352</t>
         </is>
       </c>
       <c r="B201" t="n">
-        <v>-0.002</v>
+        <v>0.0205</v>
       </c>
       <c r="C201" t="n">
-        <v>0.1981</v>
+        <v>0.3503</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>293</t>
+          <t>351</t>
         </is>
       </c>
       <c r="B202" t="n">
-        <v>-0</v>
+        <v>-0.0818</v>
       </c>
       <c r="C202" t="n">
-        <v>0.1278</v>
+        <v>0.1863</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>196</t>
         </is>
       </c>
       <c r="B203" t="n">
-        <v>-0.0033</v>
+        <v>0.2331</v>
       </c>
       <c r="C203" t="n">
-        <v>0.09569999999999999</v>
+        <v>0.803</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>296</t>
+          <t>195</t>
         </is>
       </c>
       <c r="B204" t="n">
-        <v>0.014</v>
+        <v>-0.0001</v>
       </c>
       <c r="C204" t="n">
-        <v>0.6093</v>
+        <v>0.5624</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>297</t>
+          <t>192</t>
         </is>
       </c>
       <c r="B205" t="n">
-        <v>-0.0371</v>
+        <v>0.0723</v>
       </c>
       <c r="C205" t="n">
-        <v>0.6567</v>
+        <v>0.2842</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>298</t>
+          <t>190</t>
         </is>
       </c>
       <c r="B206" t="n">
-        <v>0.0033</v>
+        <v>-0.039</v>
       </c>
       <c r="C206" t="n">
-        <v>0.368</v>
+        <v>0.2112</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>302</t>
+          <t>189</t>
         </is>
       </c>
       <c r="B207" t="n">
-        <v>-0.004</v>
+        <v>0.0823</v>
       </c>
       <c r="C207" t="n">
-        <v>0.1614</v>
+        <v>1.0237</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>303</t>
+          <t>188</t>
         </is>
       </c>
       <c r="B208" t="n">
-        <v>-0.004</v>
+        <v>-0.0226</v>
       </c>
       <c r="C208" t="n">
-        <v>0.1407</v>
+        <v>0.3139</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>187</t>
         </is>
       </c>
       <c r="B209" t="n">
-        <v>-0.022</v>
+        <v>0.0373</v>
       </c>
       <c r="C209" t="n">
-        <v>0.0965</v>
+        <v>0.7147</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>183</t>
         </is>
       </c>
       <c r="B210" t="n">
-        <v>-0.009299999999999999</v>
+        <v>-0.0356</v>
       </c>
       <c r="C210" t="n">
-        <v>0.097</v>
+        <v>0.2611</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>182</t>
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0122</v>
       </c>
       <c r="C211" t="n">
-        <v>0.127</v>
+        <v>0.4192</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>181</t>
         </is>
       </c>
       <c r="B212" t="n">
-        <v>-0.0007</v>
+        <v>-0.0067</v>
       </c>
       <c r="C212" t="n">
-        <v>0.2317</v>
+        <v>0.1714</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>308</t>
+          <t>179</t>
         </is>
       </c>
       <c r="B213" t="n">
-        <v>-0.048</v>
+        <v>-0.013</v>
       </c>
       <c r="C213" t="n">
-        <v>0.5434</v>
+        <v>0.2407</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>312</t>
+          <t>178</t>
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0.0013</v>
+        <v>0.1062</v>
       </c>
       <c r="C214" t="n">
-        <v>0.2074</v>
+        <v>0.2668</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>313</t>
+          <t>175</t>
         </is>
       </c>
       <c r="B215" t="n">
-        <v>-0.0113</v>
+        <v>-0.0123</v>
       </c>
       <c r="C215" t="n">
-        <v>0.1005</v>
+        <v>0.1031</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>174</t>
         </is>
       </c>
       <c r="B216" t="n">
-        <v>-0.0033</v>
+        <v>0.0334</v>
       </c>
       <c r="C216" t="n">
-        <v>0.6656</v>
+        <v>0.4104</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>172</t>
         </is>
       </c>
       <c r="B217" t="n">
-        <v>-0.0013</v>
+        <v>0.0259</v>
       </c>
       <c r="C217" t="n">
-        <v>0.614</v>
+        <v>0.5338000000000001</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>317</t>
+          <t>171</t>
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0.0247</v>
+        <v>0.0339</v>
       </c>
       <c r="C218" t="n">
-        <v>0.5279</v>
+        <v>0.2011</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>169</t>
         </is>
       </c>
       <c r="B219" t="n">
-        <v>-0.002</v>
+        <v>0.0074</v>
       </c>
       <c r="C219" t="n">
-        <v>0.1234</v>
+        <v>0.2799</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>168</t>
         </is>
       </c>
       <c r="B220" t="n">
-        <v>-0.0127</v>
+        <v>-0.0488</v>
       </c>
       <c r="C220" t="n">
-        <v>0.2309</v>
+        <v>0.4896</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>323</t>
+          <t>166</t>
         </is>
       </c>
       <c r="B221" t="n">
-        <v>-0.0127</v>
+        <v>0.09320000000000001</v>
       </c>
       <c r="C221" t="n">
-        <v>0.1054</v>
+        <v>0.4142</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>324</t>
+          <t>165</t>
         </is>
       </c>
       <c r="B222" t="n">
-        <v>0.018</v>
+        <v>-0.06510000000000001</v>
       </c>
       <c r="C222" t="n">
-        <v>0.3097</v>
+        <v>0.251</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>325</t>
+          <t>164</t>
         </is>
       </c>
       <c r="B223" t="n">
-        <v>-0</v>
+        <v>-0.0039</v>
       </c>
       <c r="C223" t="n">
-        <v>0.2138</v>
+        <v>0.1631</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>326</t>
+          <t>163</t>
         </is>
       </c>
       <c r="B224" t="n">
-        <v>-0.0273</v>
+        <v>-0.0002</v>
       </c>
       <c r="C224" t="n">
-        <v>0.0504</v>
+        <v>0.5504</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>328</t>
+          <t>161</t>
         </is>
       </c>
       <c r="B225" t="n">
-        <v>-0.0353</v>
+        <v>0.0716</v>
       </c>
       <c r="C225" t="n">
-        <v>0.2083</v>
+        <v>0.261</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>329</t>
+          <t>160</t>
         </is>
       </c>
       <c r="B226" t="n">
-        <v>-0.01</v>
+        <v>-0.0101</v>
       </c>
       <c r="C226" t="n">
-        <v>0.1632</v>
+        <v>0.0964</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>158</t>
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.01</v>
+        <v>-0.0363</v>
       </c>
       <c r="C227" t="n">
-        <v>0.2564</v>
+        <v>0.2019</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>331</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B228" t="n">
-        <v>-0.0013</v>
+        <v>-0.023</v>
       </c>
       <c r="C228" t="n">
-        <v>0.4849</v>
+        <v>0.2126</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>156</t>
         </is>
       </c>
       <c r="B229" t="n">
-        <v>-0.0153</v>
+        <v>0.0742</v>
       </c>
       <c r="C229" t="n">
-        <v>0.1042</v>
+        <v>0.1728</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>333</t>
+          <t>155</t>
         </is>
       </c>
       <c r="B230" t="n">
-        <v>0.0387</v>
+        <v>0.0032</v>
       </c>
       <c r="C230" t="n">
-        <v>0.4418</v>
+        <v>0.1725</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>334</t>
+          <t>154</t>
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0.0153</v>
+        <v>0.0014</v>
       </c>
       <c r="C231" t="n">
-        <v>0.2123</v>
+        <v>0.1547</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>335</t>
+          <t>153</t>
         </is>
       </c>
       <c r="B232" t="n">
-        <v>-0.0193</v>
+        <v>-0.1379</v>
       </c>
       <c r="C232" t="n">
-        <v>0.2508</v>
+        <v>0.5379</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>337</t>
+          <t>152</t>
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0.046</v>
+        <v>0.1193</v>
       </c>
       <c r="C233" t="n">
-        <v>0.5648</v>
+        <v>0.331</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>338</t>
+          <t>247</t>
         </is>
       </c>
       <c r="B234" t="n">
-        <v>0.0453</v>
+        <v>0.0259</v>
       </c>
       <c r="C234" t="n">
-        <v>0.6556</v>
+        <v>0.1323</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>245</t>
         </is>
       </c>
       <c r="B235" t="n">
-        <v>-0.0033</v>
+        <v>0.2104</v>
       </c>
       <c r="C235" t="n">
-        <v>0.57</v>
+        <v>0.1408</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>341</t>
+          <t>243</t>
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0.08</v>
+        <v>0.07290000000000001</v>
       </c>
       <c r="C236" t="n">
-        <v>0.2662</v>
+        <v>0.236</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>241</t>
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0.014</v>
+        <v>0.0148</v>
       </c>
       <c r="C237" t="n">
-        <v>0.208</v>
+        <v>0.3174</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>343</t>
+          <t>240</t>
         </is>
       </c>
       <c r="B238" t="n">
-        <v>-0.008</v>
+        <v>-0.077</v>
       </c>
       <c r="C238" t="n">
-        <v>0.2926</v>
+        <v>0.3698</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>345</t>
+          <t>239</t>
         </is>
       </c>
       <c r="B239" t="n">
-        <v>-0.004</v>
+        <v>0.0223</v>
       </c>
       <c r="C239" t="n">
-        <v>0.1245</v>
+        <v>0.4053</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>238</t>
         </is>
       </c>
       <c r="B240" t="n">
-        <v>-0.006</v>
+        <v>0.07240000000000001</v>
       </c>
       <c r="C240" t="n">
-        <v>0.0751</v>
+        <v>0.423</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>347</t>
+          <t>237</t>
         </is>
       </c>
       <c r="B241" t="n">
-        <v>-0.0373</v>
+        <v>-0.0548</v>
       </c>
       <c r="C241" t="n">
-        <v>0.3069</v>
+        <v>0.287</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>234</t>
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.0873</v>
+        <v>-0.0317</v>
       </c>
       <c r="C242" t="n">
-        <v>0.1653</v>
+        <v>0.07480000000000001</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>350</t>
+          <t>233</t>
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0.1225</v>
+        <v>-0.0402</v>
       </c>
       <c r="C243" t="n">
-        <v>1.0216</v>
+        <v>0.1228</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>351</t>
+          <t>231</t>
         </is>
       </c>
       <c r="B244" t="n">
-        <v>-0.006</v>
+        <v>-0.3102</v>
       </c>
       <c r="C244" t="n">
-        <v>0.1847</v>
+        <v>0.434</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>230</t>
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.004</v>
+        <v>0.0046</v>
       </c>
       <c r="C245" t="n">
-        <v>0.3506</v>
+        <v>0.4236</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>353</t>
+          <t>229</t>
         </is>
       </c>
       <c r="B246" t="n">
-        <v>-0.0343</v>
+        <v>-0.0697</v>
       </c>
       <c r="C246" t="n">
-        <v>0.4187</v>
+        <v>0.1841</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>354</t>
+          <t>228</t>
         </is>
       </c>
       <c r="B247" t="n">
-        <v>-0.034</v>
+        <v>0.0239</v>
       </c>
       <c r="C247" t="n">
-        <v>0.1046</v>
+        <v>0.3507</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>359</t>
+          <t>226</t>
         </is>
       </c>
       <c r="B248" t="n">
-        <v>0.006</v>
+        <v>-0.0707</v>
       </c>
       <c r="C248" t="n">
-        <v>0.2178</v>
+        <v>0.1214</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>225</t>
         </is>
       </c>
       <c r="B249" t="n">
-        <v>0.0513</v>
+        <v>-0.3359</v>
       </c>
       <c r="C249" t="n">
-        <v>0.2976</v>
+        <v>0.3753</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>224</t>
         </is>
       </c>
       <c r="B250" t="n">
-        <v>0.0033</v>
+        <v>-0.0297</v>
       </c>
       <c r="C250" t="n">
-        <v>0.5268</v>
+        <v>0.1816</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>362</t>
+          <t>223</t>
         </is>
       </c>
       <c r="B251" t="n">
-        <v>-0.0233</v>
+        <v>0.089</v>
       </c>
       <c r="C251" t="n">
-        <v>0.3575</v>
+        <v>0.0594</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>364</t>
+          <t>222</t>
         </is>
       </c>
       <c r="B252" t="n">
-        <v>0.0013</v>
+        <v>0.08550000000000001</v>
       </c>
       <c r="C252" t="n">
-        <v>0.0891</v>
+        <v>0.5541</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>367</t>
+          <t>220</t>
         </is>
       </c>
       <c r="B253" t="n">
-        <v>-0.0073</v>
+        <v>0.024</v>
       </c>
       <c r="C253" t="n">
-        <v>0.2157</v>
+        <v>0.1259</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>369</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B254" t="n">
-        <v>-0.006</v>
+        <v>-0.1084</v>
       </c>
       <c r="C254" t="n">
-        <v>0.1352</v>
+        <v>0.2093</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>370</t>
+          <t>217</t>
         </is>
       </c>
       <c r="B255" t="n">
-        <v>0.004</v>
+        <v>0.08119999999999999</v>
       </c>
       <c r="C255" t="n">
-        <v>0.1563</v>
+        <v>0.8228</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>372</t>
+          <t>216</t>
         </is>
       </c>
       <c r="B256" t="n">
-        <v>-0.0007</v>
+        <v>-0.0236</v>
       </c>
       <c r="C256" t="n">
-        <v>0.1806</v>
+        <v>0.1392</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B257" t="n">
-        <v>0.0553</v>
+        <v>0.0056</v>
       </c>
       <c r="C257" t="n">
-        <v>0.2383</v>
+        <v>0.3164</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>374</t>
+          <t>214</t>
         </is>
       </c>
       <c r="B258" t="n">
-        <v>0.0733</v>
+        <v>-0.2921</v>
       </c>
       <c r="C258" t="n">
-        <v>0.2069</v>
+        <v>0.7268</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>376</t>
+          <t>213</t>
         </is>
       </c>
       <c r="B259" t="n">
-        <v>0.0133</v>
+        <v>0.0625</v>
       </c>
       <c r="C259" t="n">
-        <v>0.1906</v>
+        <v>0.578</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>377</t>
+          <t>212</t>
         </is>
       </c>
       <c r="B260" t="n">
-        <v>-0</v>
+        <v>-0.0058</v>
       </c>
       <c r="C260" t="n">
-        <v>0.3257</v>
+        <v>0.1894</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>378</t>
+          <t>211</t>
         </is>
       </c>
       <c r="B261" t="n">
-        <v>0.0573</v>
+        <v>0.0246</v>
       </c>
       <c r="C261" t="n">
-        <v>0.3381</v>
+        <v>0.407</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>210</t>
         </is>
       </c>
       <c r="B262" t="n">
-        <v>0.02</v>
+        <v>-0.1849</v>
       </c>
       <c r="C262" t="n">
-        <v>0.1059</v>
+        <v>0.4927</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>209</t>
         </is>
       </c>
       <c r="B263" t="n">
-        <v>-0.009299999999999999</v>
+        <v>-0.1914</v>
       </c>
       <c r="C263" t="n">
-        <v>0.3833</v>
+        <v>0.4267</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>208</t>
         </is>
       </c>
       <c r="B264" t="n">
-        <v>0.0067</v>
+        <v>-0.0163</v>
       </c>
       <c r="C264" t="n">
-        <v>0.1708</v>
+        <v>0.2164</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>382</t>
+          <t>207</t>
         </is>
       </c>
       <c r="B265" t="n">
-        <v>-0.0573</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="C265" t="n">
-        <v>0.1611</v>
+        <v>0.1103</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>383</t>
+          <t>205</t>
         </is>
       </c>
       <c r="B266" t="n">
-        <v>0.004</v>
+        <v>0.0374</v>
       </c>
       <c r="C266" t="n">
-        <v>0.1862</v>
+        <v>0.2088</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>385</t>
+          <t>202</t>
         </is>
       </c>
       <c r="B267" t="n">
-        <v>-0.0273</v>
+        <v>0.0031</v>
       </c>
       <c r="C267" t="n">
-        <v>0.0506</v>
+        <v>0.1658</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>386</t>
+          <t>201</t>
         </is>
       </c>
       <c r="B268" t="n">
-        <v>-0.0127</v>
+        <v>-0.04</v>
       </c>
       <c r="C268" t="n">
-        <v>0.1014</v>
+        <v>0.162</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>387</t>
+          <t>400</t>
         </is>
       </c>
       <c r="B269" t="n">
-        <v>-0.004</v>
+        <v>0.0136</v>
       </c>
       <c r="C269" t="n">
-        <v>0.1702</v>
+        <v>0.1265</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>388</t>
+          <t>399</t>
         </is>
       </c>
       <c r="B270" t="n">
-        <v>-0.0007</v>
+        <v>0.0556</v>
       </c>
       <c r="C270" t="n">
-        <v>0.2055</v>
+        <v>0.3509</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>389</t>
+          <t>398</t>
         </is>
       </c>
       <c r="B271" t="n">
-        <v>0.0007</v>
+        <v>-0.0126</v>
       </c>
       <c r="C271" t="n">
-        <v>0.432</v>
+        <v>0.1297</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>396</t>
         </is>
       </c>
       <c r="B272" t="n">
-        <v>-0.0053</v>
+        <v>-0.0135</v>
       </c>
       <c r="C272" t="n">
-        <v>0.12</v>
+        <v>0.0814</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>391</t>
+          <t>395</t>
         </is>
       </c>
       <c r="B273" t="n">
-        <v>0.0293</v>
+        <v>0.0053</v>
       </c>
       <c r="C273" t="n">
-        <v>0.1516</v>
+        <v>0.1715</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>392</t>
+          <t>394</t>
         </is>
       </c>
       <c r="B274" t="n">
-        <v>0.016</v>
+        <v>0.1002</v>
       </c>
       <c r="C274" t="n">
-        <v>0.2023</v>
+        <v>0.1516</v>
       </c>
     </row>
     <row r="275">
@@ -4002,88 +4006,114 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>0.0113</v>
+        <v>0.09429999999999999</v>
       </c>
       <c r="C275" t="n">
-        <v>0.3238</v>
+        <v>0.3232</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>394</t>
+          <t>392</t>
         </is>
       </c>
       <c r="B276" t="n">
-        <v>0.0233</v>
+        <v>0.0029</v>
       </c>
       <c r="C276" t="n">
-        <v>0.1518</v>
+        <v>0.2025</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>395</t>
+          <t>391</t>
         </is>
       </c>
       <c r="B277" t="n">
-        <v>-0.0187</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="C277" t="n">
-        <v>0.1726</v>
+        <v>0.1519</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>396</t>
+          <t>390</t>
         </is>
       </c>
       <c r="B278" t="n">
-        <v>-0.0213</v>
+        <v>0.0275</v>
       </c>
       <c r="C278" t="n">
-        <v>0.08119999999999999</v>
+        <v>0.1196</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>398</t>
+          <t>389</t>
         </is>
       </c>
       <c r="B279" t="n">
-        <v>-0.0193</v>
+        <v>-0.0043</v>
       </c>
       <c r="C279" t="n">
-        <v>0.1297</v>
+        <v>0.4332</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>399</t>
+          <t>388</t>
         </is>
       </c>
       <c r="B280" t="n">
-        <v>0.016</v>
+        <v>0.0393</v>
       </c>
       <c r="C280" t="n">
-        <v>0.3518</v>
+        <v>0.2056</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>387</t>
         </is>
       </c>
       <c r="B281" t="n">
-        <v>-0.0067</v>
+        <v>0.0325</v>
       </c>
       <c r="C281" t="n">
-        <v>0.1267</v>
+        <v>0.1707</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>386</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>-0.0033</v>
+      </c>
+      <c r="C282" t="n">
+        <v>0.1014</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>385</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>-0.0164</v>
+      </c>
+      <c r="C283" t="n">
+        <v>0.0509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the first update in 2026.
</commit_message>
<xml_diff>
--- a/deming.xlsx
+++ b/deming.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C286"/>
+  <dimension ref="A1:C285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.0193</v>
+        <v>-0.0104</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0969</v>
+        <v>0.09669999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.014</v>
+        <v>0.0264</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0963</v>
+        <v>0.095</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.0133</v>
+        <v>-0.1468</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5499000000000001</v>
+        <v>0.5538</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.0007</v>
+        <v>0.0024</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1461</v>
+        <v>0.1463</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.022</v>
+        <v>-0.045</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1821</v>
+        <v>0.1825</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0573</v>
+        <v>0.0263</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3502</v>
+        <v>0.3508</v>
       </c>
     </row>
     <row r="8">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.0287</v>
+        <v>0.1094</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1993</v>
+        <v>0.1944</v>
       </c>
     </row>
     <row r="9">
@@ -548,10 +548,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-0.1847</v>
       </c>
       <c r="C9" t="n">
-        <v>1.25</v>
+        <v>1.2658</v>
       </c>
     </row>
     <row r="10">
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.034</v>
+        <v>-0.3189</v>
       </c>
       <c r="C10" t="n">
-        <v>0.668</v>
+        <v>0.6798999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.287</v>
+        <v>0.5809</v>
       </c>
       <c r="C11" t="n">
-        <v>0.321</v>
+        <v>0.3169</v>
       </c>
     </row>
     <row r="12">
@@ -587,10 +587,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.0173</v>
+        <v>0.07580000000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4164</v>
+        <v>0.416</v>
       </c>
     </row>
     <row r="13">
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.14</v>
+        <v>-0.0058</v>
       </c>
       <c r="C13" t="n">
-        <v>0.704</v>
+        <v>0.6984</v>
       </c>
     </row>
     <row r="14">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.106</v>
+        <v>0.1169</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6702</v>
+        <v>0.6687</v>
       </c>
     </row>
     <row r="15">
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.016</v>
+        <v>0.0495</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3869</v>
+        <v>0.3861</v>
       </c>
     </row>
     <row r="16">
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.0147</v>
+        <v>0.0606</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1721</v>
+        <v>0.1699</v>
       </c>
     </row>
     <row r="17">
@@ -652,10 +652,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0007</v>
+        <v>0.0488</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1467</v>
+        <v>0.1453</v>
       </c>
     </row>
     <row r="18">
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.1773</v>
+        <v>0.1204</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3019</v>
+        <v>0.3032</v>
       </c>
     </row>
     <row r="20">
@@ -691,10 +691,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.0707</v>
+        <v>-0.034</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3155</v>
+        <v>0.3167</v>
       </c>
     </row>
     <row r="21">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.009299999999999999</v>
+        <v>-0.0026</v>
       </c>
       <c r="C21" t="n">
         <v>0.0815</v>
@@ -717,10 +717,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.0033</v>
+        <v>-0.0121</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2852</v>
+        <v>0.2853</v>
       </c>
     </row>
     <row r="23">
@@ -730,10 +730,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.0053</v>
+        <v>0.0209</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2126</v>
+        <v>0.2125</v>
       </c>
     </row>
     <row r="24">
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.012</v>
+        <v>0.0199</v>
       </c>
       <c r="C24" t="n">
         <v>0.2106</v>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.0073</v>
+        <v>0.0973</v>
       </c>
       <c r="C25" t="n">
-        <v>0.214</v>
+        <v>0.2121</v>
       </c>
     </row>
     <row r="26">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.035</v>
+        <v>0.0128</v>
       </c>
       <c r="C26" t="n">
-        <v>0.4043</v>
+        <v>0.4058</v>
       </c>
     </row>
     <row r="27">
@@ -782,10 +782,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.0027</v>
+        <v>-0.0203</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5021</v>
+        <v>0.5027</v>
       </c>
     </row>
     <row r="28">
@@ -795,10 +795,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.0007</v>
+        <v>0.0004</v>
       </c>
       <c r="C28" t="n">
-        <v>0.212</v>
+        <v>0.2114</v>
       </c>
     </row>
     <row r="29">
@@ -808,10 +808,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.006</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1417</v>
+        <v>0.1399</v>
       </c>
     </row>
     <row r="30">
@@ -821,10 +821,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.01</v>
+        <v>0.0467</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1028</v>
+        <v>0.1022</v>
       </c>
     </row>
     <row r="31">
@@ -834,10 +834,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.03</v>
+        <v>-0.0062</v>
       </c>
       <c r="C31" t="n">
-        <v>0.3637</v>
+        <v>0.3646</v>
       </c>
     </row>
     <row r="32">
@@ -847,10 +847,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.0147</v>
+        <v>-0.01</v>
       </c>
       <c r="C32" t="n">
-        <v>0.2581</v>
+        <v>0.2578</v>
       </c>
     </row>
     <row r="33">
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.0153</v>
+        <v>0.0735</v>
       </c>
       <c r="C33" t="n">
-        <v>1.6582</v>
+        <v>1.6587</v>
       </c>
     </row>
     <row r="34">
@@ -873,10 +873,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.0107</v>
+        <v>-0.0864</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1216</v>
+        <v>0.1235</v>
       </c>
     </row>
     <row r="35">
@@ -886,10 +886,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.004</v>
+        <v>6.0122</v>
       </c>
       <c r="C35" t="n">
-        <v>0.2023</v>
+        <v>0.0697</v>
       </c>
     </row>
     <row r="36">
@@ -899,10 +899,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.0007</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="C36" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.0861</v>
       </c>
     </row>
     <row r="37">
@@ -912,10 +912,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-0.018</v>
+        <v>0.0065</v>
       </c>
       <c r="C37" t="n">
-        <v>0.4303</v>
+        <v>0.4304</v>
       </c>
     </row>
     <row r="38">
@@ -925,10 +925,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.0113</v>
+        <v>-0.2014</v>
       </c>
       <c r="C38" t="n">
-        <v>0.3976</v>
+        <v>0.4015</v>
       </c>
     </row>
     <row r="39">
@@ -938,10 +938,10 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.0033</v>
+        <v>0.0965</v>
       </c>
       <c r="C39" t="n">
-        <v>0.132</v>
+        <v>0.1292</v>
       </c>
     </row>
     <row r="40">
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-0.01</v>
+        <v>-0.009299999999999999</v>
       </c>
       <c r="C40" t="n">
         <v>0.1767</v>
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-0.028</v>
+        <v>-0.0273</v>
       </c>
       <c r="C41" t="n">
-        <v>0.309</v>
+        <v>0.3089</v>
       </c>
     </row>
     <row r="42">
@@ -977,10 +977,10 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0058</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1557</v>
+        <v>0.1558</v>
       </c>
     </row>
     <row r="43">
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-0.0013</v>
+        <v>-0.1214</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1242</v>
+        <v>0.1265</v>
       </c>
     </row>
     <row r="44">
@@ -1003,10 +1003,10 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-0.002</v>
+        <v>-0.1439</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1294</v>
+        <v>0.1327</v>
       </c>
     </row>
     <row r="45">
@@ -1016,10 +1016,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-0.002</v>
+        <v>-0.0437</v>
       </c>
       <c r="C45" t="n">
-        <v>0.2031</v>
+        <v>0.2042</v>
       </c>
     </row>
     <row r="46">
@@ -1029,7 +1029,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0056</v>
       </c>
       <c r="C46" t="n">
         <v>0.1922</v>
@@ -1042,10 +1042,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.006</v>
+        <v>0.2015</v>
       </c>
       <c r="C47" t="n">
-        <v>0.4718</v>
+        <v>0.4688</v>
       </c>
     </row>
     <row r="48">
@@ -1055,10 +1055,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-0.0033</v>
+        <v>0.0974</v>
       </c>
       <c r="C48" t="n">
-        <v>0.3355</v>
+        <v>0.3322</v>
       </c>
     </row>
     <row r="49">
@@ -1068,10 +1068,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.0273</v>
+        <v>0.0334</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2064</v>
+        <v>0.2061</v>
       </c>
     </row>
     <row r="50">
@@ -1081,10 +1081,10 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-0.0273</v>
+        <v>-0.009900000000000001</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1015</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="51">
@@ -1094,10 +1094,10 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.0133</v>
+        <v>-0.0007</v>
       </c>
       <c r="C51" t="n">
-        <v>0.281</v>
+        <v>0.2809</v>
       </c>
     </row>
     <row r="52">
@@ -1107,10 +1107,10 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0009</v>
       </c>
       <c r="C52" t="n">
-        <v>0.1927</v>
+        <v>0.1928</v>
       </c>
     </row>
     <row r="53">
@@ -1120,10 +1120,10 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-0.0107</v>
+        <v>-0.0222</v>
       </c>
       <c r="C53" t="n">
-        <v>0.2105</v>
+        <v>0.212</v>
       </c>
     </row>
     <row r="54">
@@ -1133,10 +1133,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-0.0273</v>
+        <v>-0.008</v>
       </c>
       <c r="C54" t="n">
-        <v>0.09760000000000001</v>
+        <v>0.0973</v>
       </c>
     </row>
     <row r="55">
@@ -1146,10 +1146,10 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.0213</v>
+        <v>-0.015</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1023</v>
+        <v>0.1021</v>
       </c>
     </row>
     <row r="56">
@@ -1159,10 +1159,10 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-0.005</v>
+        <v>0.0801</v>
       </c>
       <c r="C56" t="n">
-        <v>0.1027</v>
+        <v>0.09950000000000001</v>
       </c>
     </row>
     <row r="57">
@@ -1172,10 +1172,10 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>-0.008</v>
+        <v>-0.0382</v>
       </c>
       <c r="C57" t="n">
-        <v>0.4213</v>
+        <v>0.4233</v>
       </c>
     </row>
     <row r="58">
@@ -1185,10 +1185,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.0759</v>
+        <v>0.2893</v>
       </c>
       <c r="C58" t="n">
-        <v>0.5598</v>
+        <v>0.5533</v>
       </c>
     </row>
     <row r="59">
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.0233</v>
+        <v>-0.0072</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0756</v>
+        <v>0.0755</v>
       </c>
     </row>
     <row r="60">
@@ -1211,10 +1211,10 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-0.014</v>
+        <v>0.0488</v>
       </c>
       <c r="C60" t="n">
-        <v>0.2255</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="61">
@@ -1224,10 +1224,10 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-0.0047</v>
+        <v>-0.0258</v>
       </c>
       <c r="C61" t="n">
-        <v>0.1136</v>
+        <v>0.1137</v>
       </c>
     </row>
     <row r="62">
@@ -1237,10 +1237,10 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.038</v>
+        <v>0.0469</v>
       </c>
       <c r="C62" t="n">
-        <v>0.8113</v>
+        <v>0.8114</v>
       </c>
     </row>
     <row r="63">
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-0.018</v>
+        <v>-0.0168</v>
       </c>
       <c r="C63" t="n">
         <v>0.08790000000000001</v>
@@ -1263,10 +1263,10 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-0.0147</v>
+        <v>-0.0424</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1738</v>
+        <v>0.1744</v>
       </c>
     </row>
     <row r="65">
@@ -1276,10 +1276,10 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-0.008</v>
+        <v>-0.0893</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3827</v>
+        <v>0.3859</v>
       </c>
     </row>
     <row r="66">
@@ -1289,10 +1289,10 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-0.0053</v>
+        <v>-0.024</v>
       </c>
       <c r="C66" t="n">
-        <v>0.1035</v>
+        <v>0.1034</v>
       </c>
     </row>
     <row r="67">
@@ -1302,10 +1302,10 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>-0.032</v>
+        <v>-0.0437</v>
       </c>
       <c r="C67" t="n">
-        <v>0.3539</v>
+        <v>0.3542</v>
       </c>
     </row>
     <row r="68">
@@ -1315,10 +1315,10 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>-0.004</v>
+        <v>-0.016</v>
       </c>
       <c r="C68" t="n">
-        <v>0.2067</v>
+        <v>0.207</v>
       </c>
     </row>
     <row r="69">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.0467</v>
+        <v>0.0392</v>
       </c>
       <c r="C69" t="n">
-        <v>0.6322</v>
+        <v>0.6321</v>
       </c>
     </row>
     <row r="70">
@@ -1341,10 +1341,10 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>-0.0153</v>
+        <v>-0.0124</v>
       </c>
       <c r="C70" t="n">
-        <v>0.1564</v>
+        <v>0.1563</v>
       </c>
     </row>
     <row r="71">
@@ -1354,10 +1354,10 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.0953</v>
+        <v>-0.4674</v>
       </c>
       <c r="C71" t="n">
-        <v>0.6299</v>
+        <v>0.6427</v>
       </c>
     </row>
     <row r="72">
@@ -1367,10 +1367,10 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>-0.006</v>
+        <v>-0.3206</v>
       </c>
       <c r="C72" t="n">
-        <v>0.3712</v>
+        <v>0.3789</v>
       </c>
     </row>
     <row r="73">
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-0.0157</v>
+        <v>-0.0142</v>
       </c>
       <c r="C73" t="n">
         <v>0.128</v>
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-0.004</v>
+        <v>0.0193</v>
       </c>
       <c r="C74" t="n">
-        <v>0.4104</v>
+        <v>0.4111</v>
       </c>
     </row>
     <row r="75">
@@ -1406,10 +1406,10 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.075</v>
+        <v>0.0469</v>
       </c>
       <c r="C75" t="n">
-        <v>0.7471</v>
+        <v>0.7481</v>
       </c>
     </row>
     <row r="76">
@@ -1419,10 +1419,10 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>-0.013</v>
+        <v>-0.0575</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7006</v>
+        <v>0.7022</v>
       </c>
     </row>
     <row r="77">
@@ -1432,10 +1432,10 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.0468</v>
+        <v>-0.0183</v>
       </c>
       <c r="C77" t="n">
-        <v>0.3857</v>
+        <v>0.3862</v>
       </c>
     </row>
     <row r="78">
@@ -1445,7 +1445,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-0.0256</v>
+        <v>-0.0202</v>
       </c>
       <c r="C78" t="n">
         <v>0.06619999999999999</v>
@@ -1458,10 +1458,10 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-0.2295</v>
+        <v>0.0314</v>
       </c>
       <c r="C79" t="n">
-        <v>0.3977</v>
+        <v>0.4029</v>
       </c>
     </row>
     <row r="80">
@@ -1471,10 +1471,10 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.0486</v>
+        <v>-0.0357</v>
       </c>
       <c r="C80" t="n">
-        <v>0.2948</v>
+        <v>0.2973</v>
       </c>
     </row>
     <row r="81">
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-0.0115</v>
+        <v>-0.0409</v>
       </c>
       <c r="C81" t="n">
-        <v>0.3243</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="82">
@@ -1497,10 +1497,10 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.0086</v>
+        <v>-0.0206</v>
       </c>
       <c r="C82" t="n">
-        <v>0.2366</v>
+        <v>0.2369</v>
       </c>
     </row>
     <row r="83">
@@ -1510,10 +1510,10 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.3742</v>
+        <v>0.3809</v>
       </c>
       <c r="C83" t="n">
-        <v>0.3463</v>
+        <v>0.3459</v>
       </c>
     </row>
     <row r="84">
@@ -1523,10 +1523,10 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-0.0331</v>
+        <v>-0.0935</v>
       </c>
       <c r="C84" t="n">
-        <v>0.4818</v>
+        <v>0.4836</v>
       </c>
     </row>
     <row r="85">
@@ -1536,10 +1536,10 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-0.1097</v>
+        <v>-0.1942</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1277</v>
+        <v>0.1299</v>
       </c>
     </row>
     <row r="86">
@@ -1549,10 +1549,10 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>-2.2468</v>
+        <v>-0.0007</v>
       </c>
       <c r="C86" t="n">
-        <v>0.2912</v>
+        <v>0.1211</v>
       </c>
     </row>
     <row r="87">
@@ -1562,10 +1562,10 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-0.0211</v>
+        <v>0.0287</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1819</v>
+        <v>0.1812</v>
       </c>
     </row>
     <row r="88">
@@ -1584,10 +1584,10 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.011</v>
+        <v>0.0169</v>
       </c>
       <c r="C89" t="n">
-        <v>0.3348</v>
+        <v>0.3347</v>
       </c>
     </row>
     <row r="90">
@@ -1597,10 +1597,10 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-0.021</v>
+        <v>-0.0259</v>
       </c>
       <c r="C90" t="n">
-        <v>0.202</v>
+        <v>0.2025</v>
       </c>
     </row>
     <row r="91">
@@ -1610,10 +1610,10 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-0.0231</v>
+        <v>-0.0333</v>
       </c>
       <c r="C91" t="n">
-        <v>0.1215</v>
+        <v>0.1219</v>
       </c>
     </row>
     <row r="92">
@@ -1623,10 +1623,10 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>-0.0188</v>
+        <v>-0.011</v>
       </c>
       <c r="C92" t="n">
-        <v>0.2976</v>
+        <v>0.2974</v>
       </c>
     </row>
     <row r="93">
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-0.0037</v>
+        <v>0.002</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1527</v>
+        <v>0.1525</v>
       </c>
     </row>
     <row r="94">
@@ -1649,10 +1649,10 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.0485</v>
+        <v>0.0468</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1809</v>
+        <v>0.1808</v>
       </c>
     </row>
     <row r="95">
@@ -1662,10 +1662,10 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-0.0108</v>
+        <v>-0.027</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1088</v>
+        <v>0.1091</v>
       </c>
     </row>
     <row r="96">
@@ -1675,7 +1675,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-0.046</v>
+        <v>-0.0007</v>
       </c>
       <c r="C96" t="n">
         <v>0.0764</v>
@@ -1688,10 +1688,10 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-0.0214</v>
+        <v>-0.017</v>
       </c>
       <c r="C97" t="n">
-        <v>0.2114</v>
+        <v>0.2111</v>
       </c>
     </row>
     <row r="98">
@@ -1701,7 +1701,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-0.005</v>
+        <v>0.0051</v>
       </c>
       <c r="C98" t="n">
         <v>0.1721</v>
@@ -1714,10 +1714,10 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.1068</v>
+        <v>0.0742</v>
       </c>
       <c r="C99" t="n">
-        <v>0.325</v>
+        <v>0.3259</v>
       </c>
     </row>
     <row r="100">
@@ -1727,10 +1727,10 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>-0.0009</v>
+        <v>0.0289</v>
       </c>
       <c r="C100" t="n">
-        <v>0.1837</v>
+        <v>0.1831</v>
       </c>
     </row>
     <row r="101">
@@ -1740,10 +1740,10 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-0.0191</v>
+        <v>0.0151</v>
       </c>
       <c r="C101" t="n">
-        <v>0.213</v>
+        <v>0.2132</v>
       </c>
     </row>
     <row r="102">
@@ -1753,10 +1753,10 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.0022</v>
+        <v>0.0048</v>
       </c>
       <c r="C102" t="n">
-        <v>0.1023</v>
+        <v>0.1022</v>
       </c>
     </row>
     <row r="103">
@@ -1766,10 +1766,10 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.0179</v>
+        <v>0.0139</v>
       </c>
       <c r="C103" t="n">
-        <v>0.4032</v>
+        <v>0.403</v>
       </c>
     </row>
     <row r="104">
@@ -1779,10 +1779,10 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.0037</v>
+        <v>-0.0043</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1049</v>
+        <v>0.1052</v>
       </c>
     </row>
     <row r="105">
@@ -1792,10 +1792,10 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.0183</v>
+        <v>0.055</v>
       </c>
       <c r="C105" t="n">
-        <v>0.1252</v>
+        <v>0.1243</v>
       </c>
     </row>
     <row r="106">
@@ -1805,10 +1805,10 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-0.0305</v>
+        <v>-0.0403</v>
       </c>
       <c r="C106" t="n">
-        <v>0.2809</v>
+        <v>0.2812</v>
       </c>
     </row>
     <row r="107">
@@ -1818,10 +1818,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.0112</v>
+        <v>0.0243</v>
       </c>
       <c r="C107" t="n">
-        <v>0.25</v>
+        <v>0.2498</v>
       </c>
     </row>
     <row r="108">
@@ -1831,10 +1831,10 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.0405</v>
+        <v>0.0416</v>
       </c>
       <c r="C108" t="n">
-        <v>0.1745</v>
+        <v>0.1757</v>
       </c>
     </row>
     <row r="109">
@@ -1844,10 +1844,10 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-0.009299999999999999</v>
+        <v>0.001</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1016</v>
+        <v>0.1015</v>
       </c>
     </row>
     <row r="110">
@@ -1857,10 +1857,10 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>-0.0046</v>
+        <v>0.1477</v>
       </c>
       <c r="C110" t="n">
-        <v>0.3387</v>
+        <v>0.3288</v>
       </c>
     </row>
     <row r="111">
@@ -1870,10 +1870,10 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-0.0347</v>
+        <v>0.0075</v>
       </c>
       <c r="C111" t="n">
-        <v>0.538</v>
+        <v>0.5361</v>
       </c>
     </row>
     <row r="112">
@@ -1883,10 +1883,10 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-0.0323</v>
+        <v>0.0247</v>
       </c>
       <c r="C112" t="n">
-        <v>0.1557</v>
+        <v>0.1546</v>
       </c>
     </row>
     <row r="113">
@@ -1896,10 +1896,10 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>-0.0164</v>
+        <v>-0.0089</v>
       </c>
       <c r="C113" t="n">
-        <v>0.1726</v>
+        <v>0.1725</v>
       </c>
     </row>
     <row r="114">
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.0293</v>
+        <v>0.0315</v>
       </c>
       <c r="C114" t="n">
         <v>0.1734</v>
@@ -1922,10 +1922,10 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.0314</v>
+        <v>-0.008699999999999999</v>
       </c>
       <c r="C115" t="n">
-        <v>0.2113</v>
+        <v>0.2124</v>
       </c>
     </row>
     <row r="116">
@@ -1935,7 +1935,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.0017</v>
+        <v>-0.008500000000000001</v>
       </c>
       <c r="C116" t="n">
         <v>0.2016</v>
@@ -1948,7 +1948,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-0.0162</v>
+        <v>-0.0115</v>
       </c>
       <c r="C117" t="n">
         <v>0.0965</v>
@@ -1961,10 +1961,10 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.008399999999999999</v>
+        <v>0.0604</v>
       </c>
       <c r="C118" t="n">
-        <v>0.2628</v>
+        <v>0.2614</v>
       </c>
     </row>
     <row r="119">
@@ -1974,10 +1974,10 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-0.0047</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="C119" t="n">
-        <v>0.5505</v>
+        <v>0.5503</v>
       </c>
     </row>
     <row r="120">
@@ -1987,10 +1987,10 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.0053</v>
+        <v>0.0019</v>
       </c>
       <c r="C120" t="n">
-        <v>0.1631</v>
+        <v>0.163</v>
       </c>
     </row>
     <row r="121">
@@ -2000,10 +2000,10 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.0001</v>
+        <v>-0.045</v>
       </c>
       <c r="C121" t="n">
-        <v>0.2499</v>
+        <v>0.2507</v>
       </c>
     </row>
     <row r="122">
@@ -2013,10 +2013,10 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.0905</v>
+        <v>0.07829999999999999</v>
       </c>
       <c r="C122" t="n">
-        <v>0.4137</v>
+        <v>0.4143</v>
       </c>
     </row>
     <row r="123">
@@ -2026,10 +2026,10 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-0.0239</v>
+        <v>-0.046</v>
       </c>
       <c r="C123" t="n">
-        <v>0.4886</v>
+        <v>0.4898</v>
       </c>
     </row>
     <row r="124">
@@ -2039,10 +2039,10 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.0179</v>
+        <v>0.0047</v>
       </c>
       <c r="C124" t="n">
-        <v>0.2791</v>
+        <v>0.2799</v>
       </c>
     </row>
     <row r="125">
@@ -2052,10 +2052,10 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.0381</v>
+        <v>0.0151</v>
       </c>
       <c r="C125" t="n">
-        <v>0.2008</v>
+        <v>0.2012</v>
       </c>
     </row>
     <row r="126">
@@ -2065,10 +2065,10 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.0051</v>
+        <v>-0.0064</v>
       </c>
       <c r="C126" t="n">
-        <v>0.5344</v>
+        <v>0.5341</v>
       </c>
     </row>
     <row r="127">
@@ -2078,10 +2078,10 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.0408</v>
+        <v>0.0446</v>
       </c>
       <c r="C127" t="n">
-        <v>0.4105</v>
+        <v>0.4106</v>
       </c>
     </row>
     <row r="128">
@@ -2091,10 +2091,10 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0.0359</v>
+        <v>0.0077</v>
       </c>
       <c r="C128" t="n">
-        <v>0.1038</v>
+        <v>0.1028</v>
       </c>
     </row>
     <row r="129">
@@ -2104,10 +2104,10 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.09279999999999999</v>
+        <v>0.08260000000000001</v>
       </c>
       <c r="C129" t="n">
-        <v>0.2673</v>
+        <v>0.2674</v>
       </c>
     </row>
     <row r="130">
@@ -2117,10 +2117,10 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-0.0182</v>
+        <v>-0.0201</v>
       </c>
       <c r="C130" t="n">
-        <v>0.2407</v>
+        <v>0.2408</v>
       </c>
     </row>
     <row r="131">
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.0513</v>
+        <v>0.0097</v>
       </c>
       <c r="C131" t="n">
-        <v>0.1708</v>
+        <v>0.1711</v>
       </c>
     </row>
     <row r="132">
@@ -2143,10 +2143,10 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>-0.0026</v>
+        <v>-0.0027</v>
       </c>
       <c r="C132" t="n">
-        <v>0.4191</v>
+        <v>0.4193</v>
       </c>
     </row>
     <row r="133">
@@ -2156,10 +2156,10 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-0.0341</v>
+        <v>-0.0181</v>
       </c>
       <c r="C133" t="n">
-        <v>0.2614</v>
+        <v>0.2608</v>
       </c>
     </row>
     <row r="134">
@@ -2169,10 +2169,10 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.1378</v>
+        <v>0.0162</v>
       </c>
       <c r="C134" t="n">
-        <v>0.7107</v>
+        <v>0.7143</v>
       </c>
     </row>
     <row r="135">
@@ -2182,10 +2182,10 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.0617</v>
+        <v>0.0315</v>
       </c>
       <c r="C135" t="n">
-        <v>0.3122</v>
+        <v>0.3128</v>
       </c>
     </row>
     <row r="136">
@@ -2195,10 +2195,10 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.062</v>
+        <v>0.1011</v>
       </c>
       <c r="C136" t="n">
-        <v>1.0262</v>
+        <v>1.0234</v>
       </c>
     </row>
     <row r="137">
@@ -2208,10 +2208,10 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>-0.0731</v>
+        <v>-0.098</v>
       </c>
       <c r="C137" t="n">
-        <v>0.2123</v>
+        <v>0.2124</v>
       </c>
     </row>
     <row r="138">
@@ -2221,10 +2221,10 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.0031</v>
+        <v>0.0421</v>
       </c>
       <c r="C138" t="n">
-        <v>0.2853</v>
+        <v>0.2844</v>
       </c>
     </row>
     <row r="139">
@@ -2234,10 +2234,10 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>-0.0429</v>
+        <v>-0.0164</v>
       </c>
       <c r="C139" t="n">
-        <v>0.5635</v>
+        <v>0.5627</v>
       </c>
     </row>
     <row r="140">
@@ -2247,10 +2247,10 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>-0.0171</v>
+        <v>0.1719</v>
       </c>
       <c r="C140" t="n">
-        <v>0.8072</v>
+        <v>0.8027</v>
       </c>
     </row>
     <row r="141">
@@ -2260,10 +2260,10 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>-0.0452</v>
+        <v>-0.0297</v>
       </c>
       <c r="C141" t="n">
-        <v>0.1628</v>
+        <v>0.1619</v>
       </c>
     </row>
     <row r="142">
@@ -2273,10 +2273,10 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>-0.0147</v>
+        <v>-0.0015</v>
       </c>
       <c r="C142" t="n">
-        <v>0.1661</v>
+        <v>0.1658</v>
       </c>
     </row>
     <row r="143">
@@ -2286,10 +2286,10 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.0275</v>
+        <v>0.0409</v>
       </c>
       <c r="C143" t="n">
-        <v>0.2091</v>
+        <v>0.2087</v>
       </c>
     </row>
     <row r="144">
@@ -2299,10 +2299,10 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-0.0236</v>
+        <v>-0.0034</v>
       </c>
       <c r="C144" t="n">
-        <v>0.1111</v>
+        <v>0.1105</v>
       </c>
     </row>
     <row r="145">
@@ -2312,10 +2312,10 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>-0.045</v>
+        <v>-0.0432</v>
       </c>
       <c r="C145" t="n">
-        <v>0.2167</v>
+        <v>0.2168</v>
       </c>
     </row>
     <row r="146">
@@ -2325,10 +2325,10 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>-0.0044</v>
+        <v>-0.1902</v>
       </c>
       <c r="C146" t="n">
-        <v>0.4231</v>
+        <v>0.4275</v>
       </c>
     </row>
     <row r="147">
@@ -2338,10 +2338,10 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>-0.1635</v>
+        <v>-0.1353</v>
       </c>
       <c r="C147" t="n">
-        <v>0.4929</v>
+        <v>0.4922</v>
       </c>
     </row>
     <row r="148">
@@ -2351,7 +2351,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.0138</v>
+        <v>0.01</v>
       </c>
       <c r="C148" t="n">
         <v>0.4073</v>
@@ -2364,10 +2364,10 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.038</v>
+        <v>0.0148</v>
       </c>
       <c r="C149" t="n">
-        <v>0.1881</v>
+        <v>0.1887</v>
       </c>
     </row>
     <row r="150">
@@ -2377,10 +2377,10 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.0354</v>
+        <v>0.1244</v>
       </c>
       <c r="C150" t="n">
-        <v>0.5794</v>
+        <v>0.5772</v>
       </c>
     </row>
     <row r="151">
@@ -2390,10 +2390,10 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.0866</v>
+        <v>-0.3203</v>
       </c>
       <c r="C151" t="n">
-        <v>0.7198</v>
+        <v>0.7296</v>
       </c>
     </row>
     <row r="152">
@@ -2403,10 +2403,10 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>-0.0056</v>
+        <v>0.0223</v>
       </c>
       <c r="C152" t="n">
-        <v>0.3168</v>
+        <v>0.316</v>
       </c>
     </row>
     <row r="153">
@@ -2416,10 +2416,10 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>-0.0112</v>
+        <v>-0.0225</v>
       </c>
       <c r="C153" t="n">
-        <v>0.139</v>
+        <v>0.1392</v>
       </c>
     </row>
     <row r="154">
@@ -2429,10 +2429,10 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.0331</v>
+        <v>0.0328</v>
       </c>
       <c r="C154" t="n">
-        <v>0.8229</v>
+        <v>0.8228</v>
       </c>
     </row>
     <row r="155">
@@ -2442,10 +2442,10 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>-0.1579</v>
+        <v>-0.2062</v>
       </c>
       <c r="C155" t="n">
-        <v>0.2091</v>
+        <v>0.2102</v>
       </c>
     </row>
     <row r="156">
@@ -2455,10 +2455,10 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.009900000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="C156" t="n">
-        <v>0.1262</v>
+        <v>0.1259</v>
       </c>
     </row>
     <row r="157">
@@ -2481,10 +2481,10 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.0113</v>
+        <v>1.774</v>
       </c>
       <c r="C158" t="n">
-        <v>0.0607</v>
+        <v>0.0752</v>
       </c>
     </row>
     <row r="159">
@@ -2494,10 +2494,10 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>-0.0233</v>
+        <v>-0.047</v>
       </c>
       <c r="C159" t="n">
-        <v>0.181</v>
+        <v>0.1815</v>
       </c>
     </row>
     <row r="160">
@@ -2507,10 +2507,10 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>-0.0718</v>
+        <v>-0.2433</v>
       </c>
       <c r="C160" t="n">
-        <v>0.3714</v>
+        <v>0.3748</v>
       </c>
     </row>
     <row r="161">
@@ -2520,10 +2520,10 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>-0.0949</v>
+        <v>-0.098</v>
       </c>
       <c r="C161" t="n">
-        <v>0.1214</v>
+        <v>0.1218</v>
       </c>
     </row>
     <row r="162">
@@ -2533,10 +2533,10 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>-0.0741</v>
+        <v>-0.0451</v>
       </c>
       <c r="C162" t="n">
-        <v>0.352</v>
+        <v>0.3519</v>
       </c>
     </row>
     <row r="163">
@@ -2546,10 +2546,10 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>-0.0173</v>
+        <v>0.0103</v>
       </c>
       <c r="C163" t="n">
-        <v>0.1831</v>
+        <v>0.1828</v>
       </c>
     </row>
     <row r="164">
@@ -2559,10 +2559,10 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.0147</v>
+        <v>0.009599999999999999</v>
       </c>
       <c r="C164" t="n">
-        <v>0.4227</v>
+        <v>0.4229</v>
       </c>
     </row>
     <row r="165">
@@ -2572,10 +2572,10 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.0798</v>
+        <v>-0.2636</v>
       </c>
       <c r="C165" t="n">
-        <v>0.4265</v>
+        <v>0.4336</v>
       </c>
     </row>
     <row r="166">
@@ -2585,10 +2585,10 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>-0.18</v>
+        <v>-0.217</v>
       </c>
       <c r="C166" t="n">
-        <v>0.1235</v>
+        <v>0.1255</v>
       </c>
     </row>
     <row r="167">
@@ -2598,10 +2598,10 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>-0.0302</v>
+        <v>-0.031</v>
       </c>
       <c r="C167" t="n">
-        <v>0.0747</v>
+        <v>0.07480000000000001</v>
       </c>
     </row>
     <row r="168">
@@ -2611,10 +2611,10 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>-0.0711</v>
+        <v>-0.075</v>
       </c>
       <c r="C168" t="n">
-        <v>0.2872</v>
+        <v>0.2873</v>
       </c>
     </row>
     <row r="169">
@@ -2624,10 +2624,10 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>-0.009900000000000001</v>
+        <v>0.08069999999999999</v>
       </c>
       <c r="C169" t="n">
-        <v>0.4253</v>
+        <v>0.4231</v>
       </c>
     </row>
     <row r="170">
@@ -2637,10 +2637,10 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.0673</v>
+        <v>0.0344</v>
       </c>
       <c r="C170" t="n">
-        <v>0.4054</v>
+        <v>0.4049</v>
       </c>
     </row>
     <row r="171">
@@ -2650,10 +2650,10 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.0005</v>
+        <v>-0.0756</v>
       </c>
       <c r="C171" t="n">
-        <v>0.368</v>
+        <v>0.3699</v>
       </c>
     </row>
     <row r="172">
@@ -2663,10 +2663,10 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.0068</v>
+        <v>-0.0255</v>
       </c>
       <c r="C172" t="n">
-        <v>0.3177</v>
+        <v>0.3183</v>
       </c>
     </row>
     <row r="173">
@@ -2676,10 +2676,10 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.0975</v>
+        <v>0.0494</v>
       </c>
       <c r="C173" t="n">
-        <v>0.2345</v>
+        <v>0.2354</v>
       </c>
     </row>
     <row r="174">
@@ -2689,10 +2689,10 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.0169</v>
+        <v>0.197</v>
       </c>
       <c r="C174" t="n">
-        <v>0.1407</v>
+        <v>0.1408</v>
       </c>
     </row>
     <row r="175">
@@ -2702,10 +2702,10 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.0166</v>
+        <v>0.5718</v>
       </c>
       <c r="C175" t="n">
-        <v>0.1325</v>
+        <v>0.1233</v>
       </c>
     </row>
     <row r="176">
@@ -2715,7 +2715,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>-0.0023</v>
+        <v>0.0003</v>
       </c>
       <c r="C176" t="n">
         <v>0.2666</v>
@@ -2728,10 +2728,10 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.0726</v>
       </c>
       <c r="C177" t="n">
-        <v>0.2097</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="178">
@@ -2741,10 +2741,10 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.0512</v>
+        <v>0.055</v>
       </c>
       <c r="C178" t="n">
-        <v>0.2354</v>
+        <v>0.2351</v>
       </c>
     </row>
     <row r="179">
@@ -2754,10 +2754,10 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>-0.1422</v>
+        <v>-0.1377</v>
       </c>
       <c r="C179" t="n">
-        <v>0.5625</v>
+        <v>0.5656</v>
       </c>
     </row>
     <row r="180">
@@ -2767,10 +2767,10 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>0.0407</v>
+        <v>0.0344</v>
       </c>
       <c r="C180" t="n">
-        <v>0.1699</v>
+        <v>0.1701</v>
       </c>
     </row>
     <row r="181">
@@ -2780,10 +2780,10 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>-0.0699</v>
+        <v>-0.076</v>
       </c>
       <c r="C181" t="n">
-        <v>0.183</v>
+        <v>0.1829</v>
       </c>
     </row>
     <row r="182">
@@ -2793,10 +2793,10 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>-0.0397</v>
+        <v>-0.0323</v>
       </c>
       <c r="C182" t="n">
-        <v>0.4807</v>
+        <v>0.4806</v>
       </c>
     </row>
     <row r="183">
@@ -2806,10 +2806,10 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>-0.0343</v>
+        <v>-0.07580000000000001</v>
       </c>
       <c r="C183" t="n">
-        <v>0.5969</v>
+        <v>0.597</v>
       </c>
     </row>
     <row r="184">
@@ -2819,10 +2819,10 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>-0.0086</v>
+        <v>0.0091</v>
       </c>
       <c r="C184" t="n">
-        <v>0.3038</v>
+        <v>0.3034</v>
       </c>
     </row>
     <row r="185">
@@ -2832,10 +2832,10 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0.0373</v>
+        <v>0.0522</v>
       </c>
       <c r="C185" t="n">
-        <v>0.3927</v>
+        <v>0.3931</v>
       </c>
     </row>
     <row r="186">
@@ -2871,10 +2871,10 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>-0.0208</v>
+        <v>-0.0162</v>
       </c>
       <c r="C188" t="n">
-        <v>0.2953</v>
+        <v>0.2959</v>
       </c>
     </row>
     <row r="189">
@@ -2884,10 +2884,10 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>-0.0142</v>
+        <v>-0.0582</v>
       </c>
       <c r="C189" t="n">
-        <v>0.4379</v>
+        <v>0.4383</v>
       </c>
     </row>
     <row r="190">
@@ -2897,10 +2897,10 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.025</v>
+        <v>0.0038</v>
       </c>
       <c r="C190" t="n">
-        <v>0.2421</v>
+        <v>0.242</v>
       </c>
     </row>
     <row r="191">
@@ -2910,7 +2910,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>-0.048</v>
+        <v>-0.0441</v>
       </c>
       <c r="C191" t="n">
         <v>0.19</v>
@@ -2923,10 +2923,10 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>-0.0069</v>
+        <v>-0.0225</v>
       </c>
       <c r="C192" t="n">
-        <v>0.2047</v>
+        <v>0.2041</v>
       </c>
     </row>
     <row r="193">
@@ -2936,10 +2936,10 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.0692</v>
       </c>
       <c r="C193" t="n">
-        <v>0.1693</v>
+        <v>0.1625</v>
       </c>
     </row>
     <row r="194">
@@ -2949,10 +2949,10 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>-0.0012</v>
+        <v>-0.0005999999999999999</v>
       </c>
       <c r="C194" t="n">
-        <v>0.1313</v>
+        <v>0.1312</v>
       </c>
     </row>
     <row r="195">
@@ -2962,10 +2962,10 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>-0.0109</v>
+        <v>0.0007</v>
       </c>
       <c r="C195" t="n">
-        <v>0.318</v>
+        <v>0.3176</v>
       </c>
     </row>
     <row r="196">
@@ -2975,10 +2975,10 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0.0282</v>
+        <v>0.06279999999999999</v>
       </c>
       <c r="C196" t="n">
-        <v>0.2571</v>
+        <v>0.2565</v>
       </c>
     </row>
     <row r="197">
@@ -2988,10 +2988,10 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>-0.0133</v>
+        <v>-0.07920000000000001</v>
       </c>
       <c r="C197" t="n">
-        <v>0.1876</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="198">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.0043</v>
+        <v>0.0091</v>
       </c>
       <c r="C198" t="n">
         <v>0.174</v>
@@ -3014,10 +3014,10 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>-0.008200000000000001</v>
+        <v>-0.0107</v>
       </c>
       <c r="C199" t="n">
-        <v>0.1014</v>
+        <v>0.1015</v>
       </c>
     </row>
     <row r="200">
@@ -3027,10 +3027,10 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>-0.0477</v>
+        <v>0.0054</v>
       </c>
       <c r="C200" t="n">
-        <v>0.6591</v>
+        <v>0.6576</v>
       </c>
     </row>
     <row r="201">
@@ -3040,10 +3040,10 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>-0.0212</v>
+        <v>-0.0106</v>
       </c>
       <c r="C201" t="n">
-        <v>0.4826</v>
+        <v>0.4823</v>
       </c>
     </row>
     <row r="202">
@@ -3053,10 +3053,10 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>-0.0098</v>
+        <v>-0.007900000000000001</v>
       </c>
       <c r="C202" t="n">
-        <v>0.7415</v>
+        <v>0.742</v>
       </c>
     </row>
     <row r="203">
@@ -3066,7 +3066,7 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>-0.0044</v>
+        <v>-0.0038</v>
       </c>
       <c r="C203" t="n">
         <v>0.3167</v>
@@ -3079,7 +3079,7 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>-0.0077</v>
+        <v>-0.008800000000000001</v>
       </c>
       <c r="C204" t="n">
         <v>0.1982</v>
@@ -3105,10 +3105,10 @@
         </is>
       </c>
       <c r="B206" t="n">
-        <v>0.0029</v>
+        <v>-0.0181</v>
       </c>
       <c r="C206" t="n">
-        <v>0.0955</v>
+        <v>0.0958</v>
       </c>
     </row>
     <row r="207">
@@ -3118,10 +3118,10 @@
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0.0582</v>
+        <v>-0.1711</v>
       </c>
       <c r="C207" t="n">
-        <v>0.6054</v>
+        <v>0.6153999999999999</v>
       </c>
     </row>
     <row r="208">
@@ -3131,10 +3131,10 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>-0.0353</v>
+        <v>-0.033</v>
       </c>
       <c r="C208" t="n">
-        <v>0.6567</v>
+        <v>0.6566</v>
       </c>
     </row>
     <row r="209">
@@ -3144,10 +3144,10 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0.0136</v>
+        <v>-0.0005</v>
       </c>
       <c r="C209" t="n">
-        <v>0.3674</v>
+        <v>0.3678</v>
       </c>
     </row>
     <row r="210">
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="B210" t="n">
-        <v>0.0257</v>
+        <v>0.0276</v>
       </c>
       <c r="C210" t="n">
         <v>0.1608</v>
@@ -3170,10 +3170,10 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0.0189</v>
+        <v>-0.0117</v>
       </c>
       <c r="C211" t="n">
-        <v>0.1407</v>
+        <v>0.1417</v>
       </c>
     </row>
     <row r="212">
@@ -3183,10 +3183,10 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>-0.0197</v>
+        <v>-0.0172</v>
       </c>
       <c r="C212" t="n">
-        <v>0.0964</v>
+        <v>0.0963</v>
       </c>
     </row>
     <row r="213">
@@ -3196,10 +3196,10 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>-0.005</v>
+        <v>-0.0094</v>
       </c>
       <c r="C213" t="n">
-        <v>0.097</v>
+        <v>0.0974</v>
       </c>
     </row>
     <row r="214">
@@ -3209,10 +3209,10 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>-0.0047</v>
+        <v>0.018</v>
       </c>
       <c r="C214" t="n">
-        <v>0.1271</v>
+        <v>0.1262</v>
       </c>
     </row>
     <row r="215">
@@ -3222,10 +3222,10 @@
         </is>
       </c>
       <c r="B215" t="n">
-        <v>0.1013</v>
+        <v>0.1481</v>
       </c>
       <c r="C215" t="n">
-        <v>0.2295</v>
+        <v>0.2284</v>
       </c>
     </row>
     <row r="216">
@@ -3235,10 +3235,10 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>-0.0404</v>
+        <v>-0.0187</v>
       </c>
       <c r="C216" t="n">
-        <v>0.5433</v>
+        <v>0.5431</v>
       </c>
     </row>
     <row r="217">
@@ -3248,10 +3248,10 @@
         </is>
       </c>
       <c r="B217" t="n">
-        <v>0.0025</v>
+        <v>-0.0016</v>
       </c>
       <c r="C217" t="n">
-        <v>0.2074</v>
+        <v>0.2076</v>
       </c>
     </row>
     <row r="218">
@@ -3261,10 +3261,10 @@
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0.0112</v>
+        <v>-0.0626</v>
       </c>
       <c r="C218" t="n">
-        <v>0.1004</v>
+        <v>0.1029</v>
       </c>
     </row>
     <row r="219">
@@ -3274,10 +3274,10 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0.0576</v>
+        <v>-0.1443</v>
       </c>
       <c r="C219" t="n">
-        <v>0.3152</v>
+        <v>0.3189</v>
       </c>
     </row>
     <row r="220">
@@ -3287,10 +3287,10 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.0203</v>
+        <v>-0.0144</v>
       </c>
       <c r="C220" t="n">
-        <v>0.6652</v>
+        <v>0.6667999999999999</v>
       </c>
     </row>
     <row r="221">
@@ -3300,10 +3300,10 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>-0.0167</v>
+        <v>-0.0742</v>
       </c>
       <c r="C221" t="n">
-        <v>0.6172</v>
+        <v>0.6206</v>
       </c>
     </row>
     <row r="222">
@@ -3313,10 +3313,10 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>-0.0002</v>
+        <v>0.0356</v>
       </c>
       <c r="C222" t="n">
-        <v>0.5283</v>
+        <v>0.5275</v>
       </c>
     </row>
     <row r="223">
@@ -3326,10 +3326,10 @@
         </is>
       </c>
       <c r="B223" t="n">
-        <v>-0.1349</v>
+        <v>-0.0367</v>
       </c>
       <c r="C223" t="n">
-        <v>0.1261</v>
+        <v>0.1248</v>
       </c>
     </row>
     <row r="224">
@@ -3339,10 +3339,10 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>-0.0089</v>
+        <v>0.0141</v>
       </c>
       <c r="C224" t="n">
-        <v>0.2308</v>
+        <v>0.2304</v>
       </c>
     </row>
     <row r="225">
@@ -3352,10 +3352,10 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.0023</v>
+        <v>-0.0101</v>
       </c>
       <c r="C225" t="n">
-        <v>0.105</v>
+        <v>0.1052</v>
       </c>
     </row>
     <row r="226">
@@ -3365,10 +3365,10 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.0315</v>
+        <v>0.0375</v>
       </c>
       <c r="C226" t="n">
-        <v>0.3094</v>
+        <v>0.3091</v>
       </c>
     </row>
     <row r="227">
@@ -3378,10 +3378,10 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.0602</v>
+        <v>0.09470000000000001</v>
       </c>
       <c r="C227" t="n">
-        <v>0.2122</v>
+        <v>0.2102</v>
       </c>
     </row>
     <row r="228">
@@ -3391,7 +3391,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>-0.0242</v>
+        <v>-0.0246</v>
       </c>
       <c r="C228" t="n">
         <v>0.0503</v>
@@ -3404,10 +3404,10 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>-0.0026</v>
+        <v>0.0135</v>
       </c>
       <c r="C229" t="n">
-        <v>0.2079</v>
+        <v>0.2077</v>
       </c>
     </row>
     <row r="230">
@@ -3417,10 +3417,10 @@
         </is>
       </c>
       <c r="B230" t="n">
-        <v>-0.0173</v>
+        <v>0.0392</v>
       </c>
       <c r="C230" t="n">
-        <v>0.1637</v>
+        <v>0.1619</v>
       </c>
     </row>
     <row r="231">
@@ -3430,10 +3430,10 @@
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0.0258</v>
+        <v>0.0023</v>
       </c>
       <c r="C231" t="n">
-        <v>0.2558</v>
+        <v>0.2561</v>
       </c>
     </row>
     <row r="232">
@@ -3443,10 +3443,10 @@
         </is>
       </c>
       <c r="B232" t="n">
-        <v>0.0072</v>
+        <v>0.0252</v>
       </c>
       <c r="C232" t="n">
-        <v>0.4848</v>
+        <v>0.4846</v>
       </c>
     </row>
     <row r="233">
@@ -3456,10 +3456,10 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>-0.0179</v>
+        <v>-1.2121</v>
       </c>
       <c r="C233" t="n">
-        <v>0.1043</v>
+        <v>0.1769</v>
       </c>
     </row>
     <row r="234">
@@ -3482,7 +3482,7 @@
         </is>
       </c>
       <c r="B235" t="n">
-        <v>0.0098</v>
+        <v>0.0094</v>
       </c>
       <c r="C235" t="n">
         <v>0.2122</v>
@@ -3495,10 +3495,10 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>-0.0354</v>
+        <v>-0.0206</v>
       </c>
       <c r="C236" t="n">
-        <v>0.251</v>
+        <v>0.2505</v>
       </c>
     </row>
     <row r="237">
@@ -3508,10 +3508,10 @@
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0.0357</v>
+        <v>-0.0363</v>
       </c>
       <c r="C237" t="n">
-        <v>0.5649</v>
+        <v>0.5666</v>
       </c>
     </row>
     <row r="238">
@@ -3521,633 +3521,620 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.04</v>
+        <v>-0.0735</v>
       </c>
       <c r="C238" t="n">
-        <v>0.655</v>
+        <v>0.6536999999999999</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>339</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B239" t="n">
-        <v>0.0147</v>
+        <v>0.1586</v>
       </c>
       <c r="C239" t="n">
-        <v>0.1933</v>
+        <v>0.5738</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>341</t>
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.0271</v>
+        <v>0.0592</v>
       </c>
       <c r="C240" t="n">
-        <v>0.5699</v>
+        <v>0.2659</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>341</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B241" t="n">
-        <v>0.1096</v>
+        <v>0.3957</v>
       </c>
       <c r="C241" t="n">
-        <v>0.2653</v>
+        <v>0.1998</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>343</t>
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.011</v>
+        <v>-0.2405</v>
       </c>
       <c r="C242" t="n">
-        <v>0.2083</v>
+        <v>0.2965</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>343</t>
+          <t>345</t>
         </is>
       </c>
       <c r="B243" t="n">
-        <v>-0.216</v>
+        <v>0.0919</v>
       </c>
       <c r="C243" t="n">
-        <v>0.2968</v>
+        <v>0.1248</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>345</t>
+          <t>346</t>
         </is>
       </c>
       <c r="B244" t="n">
-        <v>-0.0024</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="C244" t="n">
-        <v>0.1245</v>
+        <v>0.0752</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>347</t>
         </is>
       </c>
       <c r="B245" t="n">
-        <v>-0.007900000000000001</v>
+        <v>0.0297</v>
       </c>
       <c r="C245" t="n">
-        <v>0.0751</v>
+        <v>0.3054</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>347</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B246" t="n">
-        <v>0.018</v>
+        <v>-0.0256</v>
       </c>
       <c r="C246" t="n">
-        <v>0.3057</v>
+        <v>0.1678</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>350</t>
         </is>
       </c>
       <c r="B247" t="n">
-        <v>-0.0336</v>
+        <v>0.0891</v>
       </c>
       <c r="C247" t="n">
-        <v>0.1679</v>
+        <v>1.0225</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>350</t>
+          <t>351</t>
         </is>
       </c>
       <c r="B248" t="n">
-        <v>0.1275</v>
+        <v>0.1212</v>
       </c>
       <c r="C248" t="n">
-        <v>1.0216</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>351</t>
+          <t>352</t>
         </is>
       </c>
       <c r="B249" t="n">
-        <v>-0.0576</v>
+        <v>0.0518</v>
       </c>
       <c r="C249" t="n">
-        <v>0.1858</v>
+        <v>0.3498</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>353</t>
         </is>
       </c>
       <c r="B250" t="n">
-        <v>-0.0015</v>
+        <v>0.0069</v>
       </c>
       <c r="C250" t="n">
-        <v>0.3509</v>
+        <v>0.4179</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>353</t>
+          <t>354</t>
         </is>
       </c>
       <c r="B251" t="n">
-        <v>-0.0083</v>
+        <v>-0.0322</v>
       </c>
       <c r="C251" t="n">
-        <v>0.4182</v>
+        <v>0.1045</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>354</t>
+          <t>359</t>
         </is>
       </c>
       <c r="B252" t="n">
-        <v>-0.0364</v>
+        <v>-0.0239</v>
       </c>
       <c r="C252" t="n">
-        <v>0.1046</v>
+        <v>0.2192</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>359</t>
+          <t>360</t>
         </is>
       </c>
       <c r="B253" t="n">
-        <v>0.0268</v>
+        <v>-0.02</v>
       </c>
       <c r="C253" t="n">
-        <v>0.218</v>
+        <v>0.2992</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>361</t>
         </is>
       </c>
       <c r="B254" t="n">
-        <v>-0.0101</v>
+        <v>0.0058</v>
       </c>
       <c r="C254" t="n">
-        <v>0.299</v>
+        <v>0.5266</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>362</t>
         </is>
       </c>
       <c r="B255" t="n">
-        <v>0.0008</v>
+        <v>-0.1416</v>
       </c>
       <c r="C255" t="n">
-        <v>0.5268</v>
+        <v>0.3603</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>362</t>
+          <t>364</t>
         </is>
       </c>
       <c r="B256" t="n">
-        <v>-0.103</v>
+        <v>-0.0004</v>
       </c>
       <c r="C256" t="n">
-        <v>0.3595</v>
+        <v>0.0891</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>364</t>
+          <t>367</t>
         </is>
       </c>
       <c r="B257" t="n">
-        <v>0.0026</v>
+        <v>-0.0019</v>
       </c>
       <c r="C257" t="n">
-        <v>0.0891</v>
+        <v>0.2152</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>367</t>
+          <t>369</t>
         </is>
       </c>
       <c r="B258" t="n">
-        <v>-0.09229999999999999</v>
+        <v>-0.0068</v>
       </c>
       <c r="C258" t="n">
-        <v>0.2176</v>
+        <v>0.1354</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>369</t>
+          <t>370</t>
         </is>
       </c>
       <c r="B259" t="n">
-        <v>-0.0221</v>
+        <v>0.0002</v>
       </c>
       <c r="C259" t="n">
-        <v>0.1355</v>
+        <v>0.1563</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>370</t>
+          <t>372</t>
         </is>
       </c>
       <c r="B260" t="n">
-        <v>0.0004</v>
+        <v>0.0653</v>
       </c>
       <c r="C260" t="n">
-        <v>0.1563</v>
+        <v>0.1791</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>372</t>
+          <t>373</t>
         </is>
       </c>
       <c r="B261" t="n">
-        <v>0.0263</v>
+        <v>-0.0119</v>
       </c>
       <c r="C261" t="n">
-        <v>0.1799</v>
+        <v>0.2386</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>374</t>
         </is>
       </c>
       <c r="B262" t="n">
-        <v>0.0036</v>
+        <v>0.037</v>
       </c>
       <c r="C262" t="n">
-        <v>0.2389</v>
+        <v>0.2077</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>374</t>
+          <t>376</t>
         </is>
       </c>
       <c r="B263" t="n">
-        <v>0.0377</v>
+        <v>0.0257</v>
       </c>
       <c r="C263" t="n">
-        <v>0.2077</v>
+        <v>0.1905</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>376</t>
+          <t>377</t>
         </is>
       </c>
       <c r="B264" t="n">
-        <v>0.0118</v>
+        <v>0.0098</v>
       </c>
       <c r="C264" t="n">
-        <v>0.1907</v>
+        <v>0.3257</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>377</t>
+          <t>378</t>
         </is>
       </c>
       <c r="B265" t="n">
-        <v>-0.0001</v>
+        <v>0.0023</v>
       </c>
       <c r="C265" t="n">
-        <v>0.3258</v>
+        <v>0.3389</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>378</t>
+          <t>379</t>
         </is>
       </c>
       <c r="B266" t="n">
-        <v>0.0235</v>
+        <v>0.0404</v>
       </c>
       <c r="C266" t="n">
-        <v>0.3386</v>
+        <v>0.1054</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>380</t>
         </is>
       </c>
       <c r="B267" t="n">
-        <v>0.0423</v>
+        <v>0.0209</v>
       </c>
       <c r="C267" t="n">
-        <v>0.1055</v>
+        <v>0.3829</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>381</t>
         </is>
       </c>
       <c r="B268" t="n">
-        <v>0.0028</v>
+        <v>0.0737</v>
       </c>
       <c r="C268" t="n">
-        <v>0.3832</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>382</t>
         </is>
       </c>
       <c r="B269" t="n">
-        <v>0.0557</v>
+        <v>0.0605</v>
       </c>
       <c r="C269" t="n">
-        <v>0.1695</v>
+        <v>0.1581</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>382</t>
+          <t>383</t>
         </is>
       </c>
       <c r="B270" t="n">
-        <v>-0.07199999999999999</v>
+        <v>-0.0649</v>
       </c>
       <c r="C270" t="n">
-        <v>0.161</v>
+        <v>0.1884</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>383</t>
+          <t>385</t>
         </is>
       </c>
       <c r="B271" t="n">
-        <v>-0.1129</v>
+        <v>-0.0344</v>
       </c>
       <c r="C271" t="n">
-        <v>0.1889</v>
+        <v>0.0508</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>385</t>
+          <t>386</t>
         </is>
       </c>
       <c r="B272" t="n">
-        <v>-0.0302</v>
+        <v>-0.0065</v>
       </c>
       <c r="C272" t="n">
-        <v>0.0508</v>
+        <v>0.1013</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>386</t>
+          <t>387</t>
         </is>
       </c>
       <c r="B273" t="n">
-        <v>-0.0095</v>
+        <v>-0.0034</v>
       </c>
       <c r="C273" t="n">
-        <v>0.1013</v>
+        <v>0.1704</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>387</t>
+          <t>388</t>
         </is>
       </c>
       <c r="B274" t="n">
-        <v>-0.0611</v>
+        <v>0.0153</v>
       </c>
       <c r="C274" t="n">
-        <v>0.1714</v>
+        <v>0.2054</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>388</t>
+          <t>389</t>
         </is>
       </c>
       <c r="B275" t="n">
-        <v>-0.0194</v>
+        <v>0.0255</v>
       </c>
       <c r="C275" t="n">
-        <v>0.2062</v>
+        <v>0.4315</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>389</t>
+          <t>390</t>
         </is>
       </c>
       <c r="B276" t="n">
-        <v>0.0063</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="C276" t="n">
-        <v>0.4323</v>
+        <v>0.1199</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>391</t>
         </is>
       </c>
       <c r="B277" t="n">
-        <v>0.0128</v>
+        <v>0.0245</v>
       </c>
       <c r="C277" t="n">
-        <v>0.1198</v>
+        <v>0.1517</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>391</t>
+          <t>392</t>
         </is>
       </c>
       <c r="B278" t="n">
-        <v>0.0314</v>
+        <v>0.0184</v>
       </c>
       <c r="C278" t="n">
-        <v>0.1516</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>392</t>
+          <t>393</t>
         </is>
       </c>
       <c r="B279" t="n">
-        <v>0.0146</v>
+        <v>0.003</v>
       </c>
       <c r="C279" t="n">
-        <v>0.2024</v>
+        <v>0.3242</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>393</t>
+          <t>394</t>
         </is>
       </c>
       <c r="B280" t="n">
-        <v>0.0633</v>
+        <v>0.0354</v>
       </c>
       <c r="C280" t="n">
-        <v>0.3228</v>
+        <v>0.1517</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>394</t>
+          <t>395</t>
         </is>
       </c>
       <c r="B281" t="n">
-        <v>0.0613</v>
+        <v>-0.0023</v>
       </c>
       <c r="C281" t="n">
-        <v>0.1513</v>
+        <v>0.1721</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>395</t>
+          <t>396</t>
         </is>
       </c>
       <c r="B282" t="n">
-        <v>-0.0251</v>
+        <v>-0.0254</v>
       </c>
       <c r="C282" t="n">
-        <v>0.1726</v>
+        <v>0.0815</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>396</t>
+          <t>398</t>
         </is>
       </c>
       <c r="B283" t="n">
-        <v>-0.0273</v>
+        <v>-0.0171</v>
       </c>
       <c r="C283" t="n">
-        <v>0.0815</v>
+        <v>0.1297</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>398</t>
+          <t>399</t>
         </is>
       </c>
       <c r="B284" t="n">
-        <v>-0.0075</v>
+        <v>-0.0132</v>
       </c>
       <c r="C284" t="n">
-        <v>0.1295</v>
+        <v>0.3521</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>399</t>
+          <t>400</t>
         </is>
       </c>
       <c r="B285" t="n">
-        <v>0.0293</v>
+        <v>-0.0064</v>
       </c>
       <c r="C285" t="n">
-        <v>0.3516</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="B286" t="n">
-        <v>-0.011</v>
-      </c>
-      <c r="C286" t="n">
         <v>0.1268</v>
       </c>
     </row>

</xml_diff>

<commit_message>
renew parameters in 15th Jan 2026
</commit_message>
<xml_diff>
--- a/deming.xlsx
+++ b/deming.xlsx
@@ -3898,10 +3898,10 @@
         </is>
       </c>
       <c r="B267" t="n">
-        <v>-0.0344</v>
+        <v>-0.0196</v>
       </c>
       <c r="C267" t="n">
-        <v>0.0508</v>
+        <v>0.0509</v>
       </c>
     </row>
     <row r="268">
@@ -3911,10 +3911,10 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>-0.0065</v>
+        <v>-0.0055</v>
       </c>
       <c r="C268" t="n">
-        <v>0.1013</v>
+        <v>0.1014</v>
       </c>
     </row>
     <row r="269">
@@ -3924,10 +3924,10 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>-0.0034</v>
+        <v>0.0239</v>
       </c>
       <c r="C269" t="n">
-        <v>0.1704</v>
+        <v>0.1708</v>
       </c>
     </row>
     <row r="270">
@@ -3937,10 +3937,10 @@
         </is>
       </c>
       <c r="B270" t="n">
-        <v>0.0153</v>
+        <v>0.0418</v>
       </c>
       <c r="C270" t="n">
-        <v>0.2054</v>
+        <v>0.2056</v>
       </c>
     </row>
     <row r="271">
@@ -3950,10 +3950,10 @@
         </is>
       </c>
       <c r="B271" t="n">
-        <v>0.0255</v>
+        <v>0.003</v>
       </c>
       <c r="C271" t="n">
-        <v>0.4315</v>
+        <v>0.433</v>
       </c>
     </row>
     <row r="272">
@@ -3963,10 +3963,10 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.0272</v>
       </c>
       <c r="C272" t="n">
-        <v>0.1199</v>
+        <v>0.1196</v>
       </c>
     </row>
     <row r="273">
@@ -3976,10 +3976,10 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>0.0245</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="C273" t="n">
-        <v>0.1517</v>
+        <v>0.1519</v>
       </c>
     </row>
     <row r="274">
@@ -3989,10 +3989,10 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>0.0184</v>
+        <v>0.0036</v>
       </c>
       <c r="C274" t="n">
-        <v>0.2023</v>
+        <v>0.2025</v>
       </c>
     </row>
     <row r="275">
@@ -4002,10 +4002,10 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>0.003</v>
+        <v>0.0956</v>
       </c>
       <c r="C275" t="n">
-        <v>0.3242</v>
+        <v>0.3232</v>
       </c>
     </row>
     <row r="276">
@@ -4015,10 +4015,10 @@
         </is>
       </c>
       <c r="B276" t="n">
-        <v>0.0354</v>
+        <v>0.0989</v>
       </c>
       <c r="C276" t="n">
-        <v>0.1517</v>
+        <v>0.1515</v>
       </c>
     </row>
     <row r="277">
@@ -4028,10 +4028,10 @@
         </is>
       </c>
       <c r="B277" t="n">
-        <v>-0.0023</v>
+        <v>0.0046</v>
       </c>
       <c r="C277" t="n">
-        <v>0.1721</v>
+        <v>0.1715</v>
       </c>
     </row>
     <row r="278">
@@ -4041,10 +4041,10 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>-0.0254</v>
+        <v>-0.0136</v>
       </c>
       <c r="C278" t="n">
-        <v>0.0815</v>
+        <v>0.0814</v>
       </c>
     </row>
     <row r="279">
@@ -4054,7 +4054,7 @@
         </is>
       </c>
       <c r="B279" t="n">
-        <v>-0.0171</v>
+        <v>-0.0123</v>
       </c>
       <c r="C279" t="n">
         <v>0.1297</v>
@@ -4067,10 +4067,10 @@
         </is>
       </c>
       <c r="B280" t="n">
-        <v>-0.0132</v>
+        <v>0.0504</v>
       </c>
       <c r="C280" t="n">
-        <v>0.3521</v>
+        <v>0.3509</v>
       </c>
     </row>
     <row r="281">
@@ -4080,10 +4080,10 @@
         </is>
       </c>
       <c r="B281" t="n">
-        <v>-0.0064</v>
+        <v>0.0133</v>
       </c>
       <c r="C281" t="n">
-        <v>0.1268</v>
+        <v>0.1265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified the range of outliers.
</commit_message>
<xml_diff>
--- a/deming.xlsx
+++ b/deming.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C281"/>
+  <dimension ref="A1:C285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.0104</v>
+        <v>-0.007900000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>0.09669999999999999</v>
+        <v>0.09660000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0264</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>0.095</v>
+        <v>0.09569999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.1468</v>
+        <v>-0.1591</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5538</v>
+        <v>0.5537</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0024</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1463</v>
+        <v>0.1464</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.045</v>
+        <v>-0.0223</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1825</v>
+        <v>0.1823</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0263</v>
+        <v>0.0225</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3508</v>
+        <v>0.3509</v>
       </c>
     </row>
     <row r="8">
@@ -535,3554 +535,3610 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1094</v>
+        <v>0.0631</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1944</v>
+        <v>0.1948</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.3189</v>
+        <v>-0.0431</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6798999999999999</v>
+        <v>1.2653</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.5809</v>
+        <v>0.0873</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3169</v>
+        <v>0.6674</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.07580000000000001</v>
+        <v>0.4864</v>
       </c>
       <c r="C11" t="n">
-        <v>0.416</v>
+        <v>0.3185</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.0058</v>
+        <v>0.0593</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6984</v>
+        <v>0.4162</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1169</v>
+        <v>0.032</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6687</v>
+        <v>0.6967</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0495</v>
+        <v>0.0247</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3861</v>
+        <v>0.6709000000000001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0606</v>
+        <v>0.0419</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1699</v>
+        <v>0.3861</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0488</v>
+        <v>0.0145</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1453</v>
+        <v>0.1711</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.018</v>
+        <v>0.0644</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2039</v>
+        <v>0.145</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1204</v>
+        <v>0.018</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3032</v>
+        <v>0.2039</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.034</v>
+        <v>0.1581</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3167</v>
+        <v>0.3028</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.0026</v>
+        <v>0.0008</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0815</v>
+        <v>0.3162</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.0121</v>
+        <v>0.0346</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2853</v>
+        <v>0.08119999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.0209</v>
+        <v>-0.0162</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2125</v>
+        <v>0.2853</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.0199</v>
+        <v>0.0328</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2106</v>
+        <v>0.2124</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.0973</v>
+        <v>0.0211</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2121</v>
+        <v>0.2106</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.0128</v>
+        <v>0.0447</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4058</v>
+        <v>0.2131</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.0203</v>
+        <v>-0.0011</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5027</v>
+        <v>0.4061</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.0004</v>
+        <v>-0.0124</v>
       </c>
       <c r="C27" t="n">
-        <v>0.2114</v>
+        <v>0.5024</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>38</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.06900000000000001</v>
+        <v>-0.008699999999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1399</v>
+        <v>0.2115</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.0467</v>
+        <v>0.06569999999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1022</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>40</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.0062</v>
+        <v>0.0365</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3646</v>
+        <v>0.1024</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.01</v>
+        <v>0.0302</v>
       </c>
       <c r="C31" t="n">
-        <v>0.2578</v>
+        <v>0.3646</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.0864</v>
+        <v>-0.0089</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1235</v>
+        <v>0.2578</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>6.0122</v>
+        <v>0.0844</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0697</v>
+        <v>1.6586</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.008399999999999999</v>
+        <v>-0.041</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0861</v>
+        <v>0.1227</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.0065</v>
+        <v>0.0263</v>
       </c>
       <c r="C35" t="n">
-        <v>0.4304</v>
+        <v>0.2016</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.1282</v>
+        <v>-0.021</v>
       </c>
       <c r="C36" t="n">
-        <v>0.3974</v>
+        <v>0.0862</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.0965</v>
+        <v>-0.0172</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1292</v>
+        <v>0.4304</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>51</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.009299999999999999</v>
+        <v>0.09470000000000001</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1767</v>
+        <v>0.3964</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>52</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.0273</v>
+        <v>0.0166</v>
       </c>
       <c r="C39" t="n">
-        <v>0.3089</v>
+        <v>0.1315</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.0058</v>
+        <v>-0.0207</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1558</v>
+        <v>0.1768</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-0.1214</v>
+        <v>-0.0139</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1265</v>
+        <v>0.3087</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-0.1439</v>
+        <v>0.0016</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1327</v>
+        <v>0.1558</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-0.0437</v>
+        <v>-0.0133</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2042</v>
+        <v>0.1246</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>62</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.0056</v>
+        <v>-0.0149</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1922</v>
+        <v>0.1314</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>63</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.2015</v>
+        <v>0.001</v>
       </c>
       <c r="C45" t="n">
-        <v>0.4688</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>64</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.0974</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="C46" t="n">
-        <v>0.3322</v>
+        <v>0.1921</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.0334</v>
+        <v>-0.0075</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2061</v>
+        <v>0.4722</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>66</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-0.009900000000000001</v>
+        <v>0.1698</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1011</v>
+        <v>0.3309</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>67</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>-0.0007</v>
+        <v>0.0789</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2809</v>
+        <v>0.2055</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>69</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.0009</v>
+        <v>-0.0105</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1928</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>70</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-0.0222</v>
+        <v>-0.0005999999999999999</v>
       </c>
       <c r="C51" t="n">
-        <v>0.212</v>
+        <v>0.281</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>71</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-0.008</v>
+        <v>-0.0018</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0973</v>
+        <v>0.1928</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-0.015</v>
+        <v>-0.008399999999999999</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1021</v>
+        <v>0.2121</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>74</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.0801</v>
+        <v>0.0104</v>
       </c>
       <c r="C54" t="n">
-        <v>0.09950000000000001</v>
+        <v>0.09719999999999999</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>75</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.0382</v>
+        <v>-0.0113</v>
       </c>
       <c r="C55" t="n">
-        <v>0.4233</v>
+        <v>0.102</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.2893</v>
+        <v>0.0177</v>
       </c>
       <c r="C56" t="n">
-        <v>0.5533</v>
+        <v>0.1018</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>79</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>-0.0072</v>
+        <v>0.0271</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0755</v>
+        <v>0.4217</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>80</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.0488</v>
+        <v>0.2962</v>
       </c>
       <c r="C58" t="n">
-        <v>0.224</v>
+        <v>0.5535</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>81</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.0258</v>
+        <v>-0.0043</v>
       </c>
       <c r="C59" t="n">
-        <v>0.1137</v>
+        <v>0.0755</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>82</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0469</v>
+        <v>0.0402</v>
       </c>
       <c r="C60" t="n">
-        <v>0.8114</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>83</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-0.0168</v>
+        <v>0.0165</v>
       </c>
       <c r="C61" t="n">
-        <v>0.08790000000000001</v>
+        <v>0.1131</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>87</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>-0.0424</v>
+        <v>0.0156</v>
       </c>
       <c r="C62" t="n">
-        <v>0.1744</v>
+        <v>0.8120000000000001</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>89</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-0.0893</v>
+        <v>-0.0206</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3859</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>90</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-0.024</v>
+        <v>-0.0456</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1034</v>
+        <v>0.1744</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>91</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-0.0437</v>
+        <v>-0.1172</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3542</v>
+        <v>0.3869</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>92</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-0.016</v>
+        <v>-0.0005</v>
       </c>
       <c r="C66" t="n">
-        <v>0.207</v>
+        <v>0.1034</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>95</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.0392</v>
+        <v>-0.0417</v>
       </c>
       <c r="C67" t="n">
-        <v>0.6321</v>
+        <v>0.3541</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>96</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>-0.0124</v>
+        <v>-0.0109</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1563</v>
+        <v>0.207</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>97</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-0.4674</v>
+        <v>0.0488</v>
       </c>
       <c r="C69" t="n">
-        <v>0.6427</v>
+        <v>0.6321</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>98</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>-0.3206</v>
+        <v>-0.0149</v>
       </c>
       <c r="C70" t="n">
-        <v>0.3789</v>
+        <v>0.1563</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>100</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>-0.0142</v>
+        <v>-0.4866</v>
       </c>
       <c r="C71" t="n">
-        <v>0.128</v>
+        <v>0.6428</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>101</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.0193</v>
+        <v>-0.006</v>
       </c>
       <c r="C72" t="n">
-        <v>0.4111</v>
+        <v>0.3712</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>103</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.0469</v>
+        <v>-0.0042</v>
       </c>
       <c r="C73" t="n">
-        <v>0.7481</v>
+        <v>0.1279</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>104</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-0.0575</v>
+        <v>-0.0192</v>
       </c>
       <c r="C74" t="n">
-        <v>0.7022</v>
+        <v>0.4114</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-0.0183</v>
+        <v>0.0124</v>
       </c>
       <c r="C75" t="n">
-        <v>0.3862</v>
+        <v>0.7486</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>107</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>-0.0202</v>
+        <v>-0.045</v>
       </c>
       <c r="C76" t="n">
-        <v>0.06619999999999999</v>
+        <v>0.7020999999999999</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.0314</v>
+        <v>0.01</v>
       </c>
       <c r="C77" t="n">
-        <v>0.4029</v>
+        <v>0.3862</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>111</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-0.0357</v>
+        <v>-0.0415</v>
       </c>
       <c r="C78" t="n">
-        <v>0.2973</v>
+        <v>0.06610000000000001</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>112</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-0.0409</v>
+        <v>0.0314</v>
       </c>
       <c r="C79" t="n">
-        <v>0.325</v>
+        <v>0.4029</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>114</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>-0.0206</v>
+        <v>-0.0118</v>
       </c>
       <c r="C80" t="n">
-        <v>0.2369</v>
+        <v>0.2975</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>115</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.3809</v>
+        <v>-0.0331</v>
       </c>
       <c r="C81" t="n">
-        <v>0.3459</v>
+        <v>0.3251</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>116</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-0.0935</v>
+        <v>-0.0205</v>
       </c>
       <c r="C82" t="n">
-        <v>0.4836</v>
+        <v>0.2365</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>117</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-0.1942</v>
+        <v>0.3761</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1299</v>
+        <v>0.3465</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>120</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-0.0007</v>
+        <v>-0.0779</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1211</v>
+        <v>0.4835</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>121</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.0287</v>
+        <v>-0.2423</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1812</v>
+        <v>0.1307</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr"/>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.1212</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>124</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.0169</v>
+        <v>0.015</v>
       </c>
       <c r="C87" t="n">
-        <v>0.3347</v>
+        <v>0.1818</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.0259</v>
+        <v>-0.0097</v>
       </c>
       <c r="C88" t="n">
-        <v>0.2025</v>
+        <v>0.2669</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>128</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-0.0333</v>
+        <v>0.0041</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1219</v>
+        <v>0.3349</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>129</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-0.011</v>
+        <v>-0.0123</v>
       </c>
       <c r="C90" t="n">
-        <v>0.2974</v>
+        <v>0.2025</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>130</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.002</v>
+        <v>-0.0296</v>
       </c>
       <c r="C91" t="n">
-        <v>0.1525</v>
+        <v>0.1218</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>131</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.0468</v>
+        <v>-0.0037</v>
       </c>
       <c r="C92" t="n">
-        <v>0.1808</v>
+        <v>0.2977</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>132</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-0.027</v>
+        <v>0.0451</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1091</v>
+        <v>0.1516</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-0.0007</v>
+        <v>0.0403</v>
       </c>
       <c r="C94" t="n">
-        <v>0.0764</v>
+        <v>0.1811</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>134</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-0.017</v>
+        <v>-0.0064</v>
       </c>
       <c r="C95" t="n">
-        <v>0.2111</v>
+        <v>0.1089</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>135</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.0051</v>
+        <v>-0.0004</v>
       </c>
       <c r="C96" t="n">
-        <v>0.1721</v>
+        <v>0.0764</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>136</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.0742</v>
+        <v>-0.0083</v>
       </c>
       <c r="C97" t="n">
-        <v>0.3259</v>
+        <v>0.2111</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>137</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.0289</v>
+        <v>0.0002</v>
       </c>
       <c r="C98" t="n">
-        <v>0.1831</v>
+        <v>0.1722</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>138</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.0171</v>
+        <v>0.06710000000000001</v>
       </c>
       <c r="C99" t="n">
-        <v>0.213</v>
+        <v>0.326</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>139</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.0048</v>
+        <v>0.0299</v>
       </c>
       <c r="C100" t="n">
-        <v>0.1022</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>140</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.0139</v>
+        <v>-0.0188</v>
       </c>
       <c r="C101" t="n">
-        <v>0.403</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>141</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>-0.0043</v>
+        <v>0.0035</v>
       </c>
       <c r="C102" t="n">
-        <v>0.1052</v>
+        <v>0.1022</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>142</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.055</v>
+        <v>0.0264</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1243</v>
+        <v>0.4026</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>143</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>-0.0403</v>
+        <v>-0.0005</v>
       </c>
       <c r="C104" t="n">
-        <v>0.2812</v>
+        <v>0.1051</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>145</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.0243</v>
+        <v>0.0521</v>
       </c>
       <c r="C105" t="n">
-        <v>0.2498</v>
+        <v>0.1243</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>146</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.0416</v>
+        <v>-0.0358</v>
       </c>
       <c r="C106" t="n">
-        <v>0.1757</v>
+        <v>0.281</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>147</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.001</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="C107" t="n">
-        <v>0.1015</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>148</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.1477</v>
+        <v>0.07770000000000001</v>
       </c>
       <c r="C108" t="n">
-        <v>0.3288</v>
+        <v>0.1755</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>149</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.0075</v>
+        <v>0.0095</v>
       </c>
       <c r="C109" t="n">
-        <v>0.5361</v>
+        <v>0.1015</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>152</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.0247</v>
+        <v>-0.0271</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1546</v>
+        <v>0.3399</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>153</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-0.0089</v>
+        <v>-0.018</v>
       </c>
       <c r="C111" t="n">
-        <v>0.1725</v>
+        <v>0.5371</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>154</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.0315</v>
+        <v>0.0147</v>
       </c>
       <c r="C112" t="n">
-        <v>0.1734</v>
+        <v>0.1546</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>155</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>-0.008699999999999999</v>
+        <v>-0.0054</v>
       </c>
       <c r="C113" t="n">
-        <v>0.2124</v>
+        <v>0.1725</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>158</t>
+          <t>156</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-0.008500000000000001</v>
+        <v>0.0224</v>
       </c>
       <c r="C114" t="n">
-        <v>0.2016</v>
+        <v>0.1735</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-0.0115</v>
+        <v>-0.0003</v>
       </c>
       <c r="C115" t="n">
-        <v>0.0965</v>
+        <v>0.2124</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>161</t>
+          <t>158</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.0604</v>
+        <v>-0.0165</v>
       </c>
       <c r="C116" t="n">
-        <v>0.2614</v>
+        <v>0.2016</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>160</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.008999999999999999</v>
+        <v>-0.0055</v>
       </c>
       <c r="C117" t="n">
-        <v>0.5503</v>
+        <v>0.0964</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>164</t>
+          <t>161</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.0019</v>
+        <v>0.0061</v>
       </c>
       <c r="C118" t="n">
-        <v>0.163</v>
+        <v>0.2628</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>163</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-0.045</v>
+        <v>0.0066</v>
       </c>
       <c r="C119" t="n">
-        <v>0.2507</v>
+        <v>0.5503</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>164</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.07829999999999999</v>
+        <v>-0.001</v>
       </c>
       <c r="C120" t="n">
-        <v>0.4143</v>
+        <v>0.163</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>165</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.046</v>
+        <v>-0.0361</v>
       </c>
       <c r="C121" t="n">
-        <v>0.4898</v>
+        <v>0.2506</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>166</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.0047</v>
+        <v>0.0914</v>
       </c>
       <c r="C122" t="n">
-        <v>0.2799</v>
+        <v>0.4142</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>171</t>
+          <t>168</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.0151</v>
+        <v>-0.0308</v>
       </c>
       <c r="C123" t="n">
-        <v>0.2012</v>
+        <v>0.4898</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>169</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-0.0064</v>
+        <v>-0.0069</v>
       </c>
       <c r="C124" t="n">
-        <v>0.5341</v>
+        <v>0.2799</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>171</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.0446</v>
+        <v>0.023</v>
       </c>
       <c r="C125" t="n">
-        <v>0.4106</v>
+        <v>0.2012</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>172</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>0.0077</v>
+        <v>-0.0062</v>
       </c>
       <c r="C126" t="n">
-        <v>0.1028</v>
+        <v>0.5342</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>174</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.08260000000000001</v>
+        <v>0.0412</v>
       </c>
       <c r="C127" t="n">
-        <v>0.2674</v>
+        <v>0.4103</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>179</t>
+          <t>175</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0.0201</v>
+        <v>-0.01</v>
       </c>
       <c r="C128" t="n">
-        <v>0.2408</v>
+        <v>0.1033</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>178</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.0097</v>
+        <v>0.1022</v>
       </c>
       <c r="C129" t="n">
-        <v>0.1711</v>
+        <v>0.2672</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>179</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-0.0027</v>
+        <v>-0.018</v>
       </c>
       <c r="C130" t="n">
-        <v>0.4193</v>
+        <v>0.2408</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>183</t>
+          <t>181</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>-0.0181</v>
+        <v>0.0496</v>
       </c>
       <c r="C131" t="n">
-        <v>0.2608</v>
+        <v>0.1706</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>182</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.0162</v>
+        <v>0.0255</v>
       </c>
       <c r="C132" t="n">
-        <v>0.7143</v>
+        <v>0.4191</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>188</t>
+          <t>183</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.0315</v>
+        <v>-0.0311</v>
       </c>
       <c r="C133" t="n">
-        <v>0.3128</v>
+        <v>0.2609</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>187</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>-0.098</v>
+        <v>0.0512</v>
       </c>
       <c r="C134" t="n">
-        <v>0.2124</v>
+        <v>0.7147</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>188</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.0421</v>
+        <v>-0.0185</v>
       </c>
       <c r="C135" t="n">
-        <v>0.2844</v>
+        <v>0.3137</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>189</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>-0.0164</v>
+        <v>0.0901</v>
       </c>
       <c r="C136" t="n">
-        <v>0.5627</v>
+        <v>1.0235</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>196</t>
+          <t>190</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.1719</v>
+        <v>-0.0121</v>
       </c>
       <c r="C137" t="n">
-        <v>0.8027</v>
+        <v>0.2111</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>192</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>-0.0297</v>
+        <v>0.081</v>
       </c>
       <c r="C138" t="n">
-        <v>0.1619</v>
+        <v>0.2841</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>202</t>
+          <t>195</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>-0.0015</v>
+        <v>-0.009900000000000001</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1658</v>
+        <v>0.5624</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>196</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.0409</v>
+        <v>0.1697</v>
       </c>
       <c r="C140" t="n">
-        <v>0.2087</v>
+        <v>0.8034</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>201</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>-0.0034</v>
+        <v>-0.0385</v>
       </c>
       <c r="C141" t="n">
-        <v>0.1105</v>
+        <v>0.162</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>202</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>-0.0432</v>
+        <v>0.0116</v>
       </c>
       <c r="C142" t="n">
-        <v>0.2168</v>
+        <v>0.1658</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>205</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>-0.1902</v>
+        <v>0.0274</v>
       </c>
       <c r="C143" t="n">
-        <v>0.4275</v>
+        <v>0.2088</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>207</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-0.1353</v>
+        <v>0.0157</v>
       </c>
       <c r="C144" t="n">
-        <v>0.4922</v>
+        <v>0.1103</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>208</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.01</v>
+        <v>-0.0294</v>
       </c>
       <c r="C145" t="n">
-        <v>0.4073</v>
+        <v>0.2167</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>209</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.0148</v>
+        <v>-0.1401</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1887</v>
+        <v>0.4266</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>210</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.1244</v>
+        <v>-0.112</v>
       </c>
       <c r="C147" t="n">
-        <v>0.5772</v>
+        <v>0.4922</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>211</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>-0.3203</v>
+        <v>0.0022</v>
       </c>
       <c r="C148" t="n">
-        <v>0.7296</v>
+        <v>0.4074</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>212</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.0223</v>
+        <v>0.002</v>
       </c>
       <c r="C149" t="n">
-        <v>0.316</v>
+        <v>0.1894</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>213</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>-0.0225</v>
+        <v>0.0547</v>
       </c>
       <c r="C150" t="n">
-        <v>0.1392</v>
+        <v>0.5796</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>214</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.0328</v>
+        <v>-0.103</v>
       </c>
       <c r="C151" t="n">
-        <v>0.8228</v>
+        <v>0.7257</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>-0.2062</v>
+        <v>0.0128</v>
       </c>
       <c r="C152" t="n">
-        <v>0.2102</v>
+        <v>0.3164</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>216</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>0.0195</v>
+        <v>-0.0299</v>
       </c>
       <c r="C153" t="n">
-        <v>0.1259</v>
+        <v>0.1392</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>217</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>-0.0502</v>
+        <v>0.0285</v>
       </c>
       <c r="C154" t="n">
-        <v>0.5567</v>
+        <v>0.8229</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>1.774</v>
+        <v>-0.1263</v>
       </c>
       <c r="C155" t="n">
-        <v>0.0752</v>
+        <v>0.2094</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>220</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>-0.047</v>
+        <v>0.0225</v>
       </c>
       <c r="C156" t="n">
-        <v>0.1815</v>
+        <v>0.1259</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>222</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>-0.2433</v>
+        <v>0.0423</v>
       </c>
       <c r="C157" t="n">
-        <v>0.3748</v>
+        <v>0.555</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>226</t>
+          <t>223</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>-0.098</v>
+        <v>0.0716</v>
       </c>
       <c r="C158" t="n">
-        <v>0.1218</v>
+        <v>0.0597</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>228</t>
+          <t>224</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>-0.0451</v>
+        <v>-0.0244</v>
       </c>
       <c r="C159" t="n">
-        <v>0.3519</v>
+        <v>0.1815</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>229</t>
+          <t>225</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.0103</v>
+        <v>-0.2709</v>
       </c>
       <c r="C160" t="n">
-        <v>0.1828</v>
+        <v>0.3751</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>226</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.009599999999999999</v>
+        <v>-0.0589</v>
       </c>
       <c r="C161" t="n">
-        <v>0.4229</v>
+        <v>0.1214</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>228</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>-0.2636</v>
+        <v>-0.0106</v>
       </c>
       <c r="C162" t="n">
-        <v>0.4336</v>
+        <v>0.3517</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>233</t>
+          <t>229</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>-0.217</v>
+        <v>-0.0376</v>
       </c>
       <c r="C163" t="n">
-        <v>0.1255</v>
+        <v>0.1841</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>234</t>
+          <t>230</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>-0.031</v>
+        <v>0.0007</v>
       </c>
       <c r="C164" t="n">
-        <v>0.07480000000000001</v>
+        <v>0.4231</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>237</t>
+          <t>231</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>-0.075</v>
+        <v>-0.2346</v>
       </c>
       <c r="C165" t="n">
-        <v>0.2873</v>
+        <v>0.4337</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>233</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.08069999999999999</v>
+        <v>0.0228</v>
       </c>
       <c r="C166" t="n">
-        <v>0.4231</v>
+        <v>0.1229</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>234</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.0344</v>
+        <v>-0.0335</v>
       </c>
       <c r="C167" t="n">
-        <v>0.4049</v>
+        <v>0.07480000000000001</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>237</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>-0.0756</v>
+        <v>-0.0529</v>
       </c>
       <c r="C168" t="n">
-        <v>0.3699</v>
+        <v>0.2872</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>238</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>-0.0255</v>
+        <v>0.0111</v>
       </c>
       <c r="C169" t="n">
-        <v>0.3183</v>
+        <v>0.4246</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>239</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.0494</v>
+        <v>0.0743</v>
       </c>
       <c r="C170" t="n">
-        <v>0.2354</v>
+        <v>0.405</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>240</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.197</v>
+        <v>-0.0576</v>
       </c>
       <c r="C171" t="n">
-        <v>0.1408</v>
+        <v>0.3697</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>241</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.5718</v>
+        <v>0.0092</v>
       </c>
       <c r="C172" t="n">
-        <v>0.1233</v>
+        <v>0.3174</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>243</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.0003</v>
+        <v>0.06419999999999999</v>
       </c>
       <c r="C173" t="n">
-        <v>0.2666</v>
+        <v>0.236</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>245</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.0726</v>
+        <v>0.1893</v>
       </c>
       <c r="C174" t="n">
-        <v>0.21</v>
+        <v>0.1409</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>253</t>
+          <t>247</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.055</v>
+        <v>0.0154</v>
       </c>
       <c r="C175" t="n">
-        <v>0.2351</v>
+        <v>0.1324</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>251</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>-0.1377</v>
+        <v>0.0209</v>
       </c>
       <c r="C176" t="n">
-        <v>0.5656</v>
+        <v>0.2666</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>252</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.0344</v>
+        <v>0.07439999999999999</v>
       </c>
       <c r="C177" t="n">
-        <v>0.1701</v>
+        <v>0.2101</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>253</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>-0.076</v>
+        <v>0.0582</v>
       </c>
       <c r="C178" t="n">
-        <v>0.1829</v>
+        <v>0.2351</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>257</t>
+          <t>254</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>-0.0323</v>
+        <v>0.0863</v>
       </c>
       <c r="C179" t="n">
-        <v>0.4806</v>
+        <v>0.5668</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>255</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>-0.07580000000000001</v>
+        <v>0.0245</v>
       </c>
       <c r="C180" t="n">
-        <v>0.597</v>
+        <v>0.1699</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>260</t>
+          <t>256</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>0.0091</v>
+        <v>-0.0621</v>
       </c>
       <c r="C181" t="n">
-        <v>0.3034</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>261</t>
+          <t>257</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.0522</v>
+        <v>-0.022</v>
       </c>
       <c r="C182" t="n">
-        <v>0.3931</v>
+        <v>0.4803</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>262</t>
+          <t>258</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.16</v>
+        <v>0.0031</v>
       </c>
       <c r="C183" t="n">
-        <v>0.09</v>
+        <v>0.5952</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>263</t>
+          <t>260</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0.0167</v>
+        <v>-0.002</v>
       </c>
       <c r="C184" t="n">
-        <v>0.2048</v>
+        <v>0.3036</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>264</t>
+          <t>261</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>-0.0162</v>
+        <v>0.158</v>
       </c>
       <c r="C185" t="n">
-        <v>0.2959</v>
+        <v>0.3924</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>266</t>
+          <t>262</t>
         </is>
       </c>
       <c r="B186" t="n">
-        <v>-0.0582</v>
+        <v>0.0051</v>
       </c>
       <c r="C186" t="n">
-        <v>0.4383</v>
+        <v>0.1008</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>263</t>
         </is>
       </c>
       <c r="B187" t="n">
-        <v>0.0038</v>
+        <v>0.07049999999999999</v>
       </c>
       <c r="C187" t="n">
-        <v>0.242</v>
+        <v>0.2037</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>271</t>
+          <t>264</t>
         </is>
       </c>
       <c r="B188" t="n">
-        <v>-0.0441</v>
+        <v>-0.0185</v>
       </c>
       <c r="C188" t="n">
-        <v>0.19</v>
+        <v>0.2959</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>274</t>
+          <t>266</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>-0.0225</v>
+        <v>0.0503</v>
       </c>
       <c r="C189" t="n">
-        <v>0.2041</v>
+        <v>0.4373</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>275</t>
+          <t>267</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.067</v>
+        <v>0.0283</v>
       </c>
       <c r="C190" t="n">
-        <v>0.1626</v>
+        <v>0.2418</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>276</t>
+          <t>271</t>
         </is>
       </c>
       <c r="B191" t="n">
-        <v>-0.0005999999999999999</v>
+        <v>0.0241</v>
       </c>
       <c r="C191" t="n">
-        <v>0.1312</v>
+        <v>0.1897</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>274</t>
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.0007</v>
+        <v>-0.0276</v>
       </c>
       <c r="C192" t="n">
-        <v>0.3176</v>
+        <v>0.2041</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>279</t>
+          <t>275</t>
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.06279999999999999</v>
+        <v>0.0516</v>
       </c>
       <c r="C193" t="n">
-        <v>0.2565</v>
+        <v>0.1631</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>280</t>
+          <t>276</t>
         </is>
       </c>
       <c r="B194" t="n">
-        <v>-0.07920000000000001</v>
+        <v>-0.001</v>
       </c>
       <c r="C194" t="n">
-        <v>0.189</v>
+        <v>0.1312</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>281</t>
+          <t>278</t>
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0.0091</v>
+        <v>-0.0031</v>
       </c>
       <c r="C195" t="n">
-        <v>0.174</v>
+        <v>0.3176</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>279</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>-0.0107</v>
+        <v>0.0629</v>
       </c>
       <c r="C196" t="n">
-        <v>0.1015</v>
+        <v>0.2567</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>287</t>
+          <t>280</t>
         </is>
       </c>
       <c r="B197" t="n">
-        <v>0.0054</v>
+        <v>-0.08799999999999999</v>
       </c>
       <c r="C197" t="n">
-        <v>0.6576</v>
+        <v>0.1898</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>288</t>
+          <t>281</t>
         </is>
       </c>
       <c r="B198" t="n">
-        <v>-0.0106</v>
+        <v>0.0103</v>
       </c>
       <c r="C198" t="n">
-        <v>0.4823</v>
+        <v>0.1739</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>284</t>
         </is>
       </c>
       <c r="B199" t="n">
-        <v>-0.007900000000000001</v>
+        <v>-0.0116</v>
       </c>
       <c r="C199" t="n">
-        <v>0.742</v>
+        <v>0.1015</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>291</t>
+          <t>287</t>
         </is>
       </c>
       <c r="B200" t="n">
-        <v>-0.0038</v>
+        <v>0.0201</v>
       </c>
       <c r="C200" t="n">
-        <v>0.3167</v>
+        <v>0.6573</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>292</t>
+          <t>288</t>
         </is>
       </c>
       <c r="B201" t="n">
-        <v>-0.008800000000000001</v>
+        <v>0.035</v>
       </c>
       <c r="C201" t="n">
-        <v>0.1982</v>
+        <v>0.4822</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>293</t>
+          <t>290</t>
         </is>
       </c>
       <c r="B202" t="n">
-        <v>-0.0042</v>
+        <v>0.0046</v>
       </c>
       <c r="C202" t="n">
-        <v>0.1279</v>
+        <v>0.7417</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>291</t>
         </is>
       </c>
       <c r="B203" t="n">
-        <v>-0.0181</v>
+        <v>0.0055</v>
       </c>
       <c r="C203" t="n">
-        <v>0.0958</v>
+        <v>0.3166</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>296</t>
+          <t>292</t>
         </is>
       </c>
       <c r="B204" t="n">
-        <v>-0.1711</v>
+        <v>0.0007</v>
       </c>
       <c r="C204" t="n">
-        <v>0.6153999999999999</v>
+        <v>0.1981</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>297</t>
+          <t>293</t>
         </is>
       </c>
       <c r="B205" t="n">
-        <v>-0.033</v>
+        <v>-0.0034</v>
       </c>
       <c r="C205" t="n">
-        <v>0.6566</v>
+        <v>0.1278</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>298</t>
+          <t>295</t>
         </is>
       </c>
       <c r="B206" t="n">
-        <v>-0.0005</v>
+        <v>-0.0067</v>
       </c>
       <c r="C206" t="n">
-        <v>0.3678</v>
+        <v>0.09569999999999999</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>302</t>
+          <t>296</t>
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0.0276</v>
+        <v>-0.2973</v>
       </c>
       <c r="C207" t="n">
-        <v>0.1608</v>
+        <v>0.6165</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>303</t>
+          <t>297</t>
         </is>
       </c>
       <c r="B208" t="n">
-        <v>-0.0117</v>
+        <v>-0.0182</v>
       </c>
       <c r="C208" t="n">
-        <v>0.1417</v>
+        <v>0.6559</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>298</t>
         </is>
       </c>
       <c r="B209" t="n">
-        <v>-0.0172</v>
+        <v>-0.0065</v>
       </c>
       <c r="C209" t="n">
-        <v>0.0963</v>
+        <v>0.3678</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>302</t>
         </is>
       </c>
       <c r="B210" t="n">
-        <v>-0.0094</v>
+        <v>0.0325</v>
       </c>
       <c r="C210" t="n">
-        <v>0.0974</v>
+        <v>0.1606</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>303</t>
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0.018</v>
+        <v>0.0112</v>
       </c>
       <c r="C211" t="n">
-        <v>0.1262</v>
+        <v>0.1418</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>304</t>
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0.1481</v>
+        <v>-0.0105</v>
       </c>
       <c r="C212" t="n">
-        <v>0.2284</v>
+        <v>0.09619999999999999</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>308</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B213" t="n">
-        <v>-0.0187</v>
+        <v>-0.0044</v>
       </c>
       <c r="C213" t="n">
-        <v>0.5431</v>
+        <v>0.0974</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>312</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B214" t="n">
-        <v>-0.0016</v>
+        <v>0.0143</v>
       </c>
       <c r="C214" t="n">
-        <v>0.2076</v>
+        <v>0.1262</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>313</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B215" t="n">
-        <v>-0.0626</v>
+        <v>0.1023</v>
       </c>
       <c r="C215" t="n">
-        <v>0.1029</v>
+        <v>0.2297</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>314</t>
+          <t>308</t>
         </is>
       </c>
       <c r="B216" t="n">
-        <v>-0.1443</v>
+        <v>-0.007900000000000001</v>
       </c>
       <c r="C216" t="n">
-        <v>0.3189</v>
+        <v>0.5431</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>312</t>
         </is>
       </c>
       <c r="B217" t="n">
-        <v>-0.0144</v>
+        <v>-0.0008</v>
       </c>
       <c r="C217" t="n">
-        <v>0.6667999999999999</v>
+        <v>0.2077</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>313</t>
         </is>
       </c>
       <c r="B218" t="n">
-        <v>-0.0742</v>
+        <v>0.028</v>
       </c>
       <c r="C218" t="n">
-        <v>0.6206</v>
+        <v>0.1024</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>317</t>
+          <t>314</t>
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0.0356</v>
+        <v>-0.0158</v>
       </c>
       <c r="C219" t="n">
-        <v>0.5275</v>
+        <v>0.3174</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>315</t>
         </is>
       </c>
       <c r="B220" t="n">
-        <v>-0.0367</v>
+        <v>-0.0842</v>
       </c>
       <c r="C220" t="n">
-        <v>0.1248</v>
+        <v>0.6687</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>316</t>
         </is>
       </c>
       <c r="B221" t="n">
-        <v>0.0141</v>
+        <v>-0.0677</v>
       </c>
       <c r="C221" t="n">
-        <v>0.2304</v>
+        <v>0.6233</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>323</t>
+          <t>317</t>
         </is>
       </c>
       <c r="B222" t="n">
-        <v>-0.0101</v>
+        <v>0.0609</v>
       </c>
       <c r="C222" t="n">
-        <v>0.1052</v>
+        <v>0.5271</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>324</t>
+          <t>319</t>
         </is>
       </c>
       <c r="B223" t="n">
-        <v>0.0375</v>
+        <v>-0.0308</v>
       </c>
       <c r="C223" t="n">
-        <v>0.3091</v>
+        <v>0.1254</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>325</t>
+          <t>320</t>
         </is>
       </c>
       <c r="B224" t="n">
-        <v>0.09470000000000001</v>
+        <v>-0.0174</v>
       </c>
       <c r="C224" t="n">
-        <v>0.2102</v>
+        <v>0.2309</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>326</t>
+          <t>323</t>
         </is>
       </c>
       <c r="B225" t="n">
-        <v>-0.0246</v>
+        <v>0.0151</v>
       </c>
       <c r="C225" t="n">
-        <v>0.0503</v>
+        <v>0.1048</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>328</t>
+          <t>324</t>
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.0135</v>
+        <v>0.0392</v>
       </c>
       <c r="C226" t="n">
-        <v>0.2077</v>
+        <v>0.3092</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>329</t>
+          <t>325</t>
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.0392</v>
+        <v>0.1647</v>
       </c>
       <c r="C227" t="n">
-        <v>0.1619</v>
+        <v>0.2095</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>326</t>
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.0023</v>
+        <v>-0.0122</v>
       </c>
       <c r="C228" t="n">
-        <v>0.2561</v>
+        <v>0.0502</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>331</t>
+          <t>328</t>
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0.0252</v>
+        <v>0.0335</v>
       </c>
       <c r="C229" t="n">
-        <v>0.4846</v>
+        <v>0.2075</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>329</t>
         </is>
       </c>
       <c r="B230" t="n">
-        <v>-1.2121</v>
+        <v>0.0466</v>
       </c>
       <c r="C230" t="n">
-        <v>0.1769</v>
+        <v>0.1619</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>333</t>
+          <t>330</t>
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0.0269</v>
+        <v>-0.0025</v>
       </c>
       <c r="C231" t="n">
-        <v>0.4418</v>
+        <v>0.2561</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>334</t>
+          <t>331</t>
         </is>
       </c>
       <c r="B232" t="n">
-        <v>0.0094</v>
+        <v>0.0141</v>
       </c>
       <c r="C232" t="n">
-        <v>0.2122</v>
+        <v>0.4848</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>335</t>
+          <t>332</t>
         </is>
       </c>
       <c r="B233" t="n">
-        <v>-0.0206</v>
+        <v>0.0524</v>
       </c>
       <c r="C233" t="n">
-        <v>0.2505</v>
+        <v>0.1033</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>337</t>
+          <t>333</t>
         </is>
       </c>
       <c r="B234" t="n">
-        <v>-0.0363</v>
+        <v>0.0425</v>
       </c>
       <c r="C234" t="n">
-        <v>0.5666</v>
+        <v>0.4416</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>338</t>
+          <t>334</t>
         </is>
       </c>
       <c r="B235" t="n">
-        <v>-0.0735</v>
+        <v>0.0046</v>
       </c>
       <c r="C235" t="n">
-        <v>0.6536999999999999</v>
+        <v>0.2123</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>335</t>
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0.1586</v>
+        <v>-0.0263</v>
       </c>
       <c r="C236" t="n">
-        <v>0.5738</v>
+        <v>0.2505</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>341</t>
+          <t>337</t>
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0.0592</v>
+        <v>-0.0322</v>
       </c>
       <c r="C237" t="n">
-        <v>0.2659</v>
+        <v>0.5664</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>338</t>
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.3957</v>
+        <v>-0.1239</v>
       </c>
       <c r="C238" t="n">
-        <v>0.1998</v>
+        <v>0.654</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>343</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B239" t="n">
-        <v>-0.2405</v>
+        <v>0.1725</v>
       </c>
       <c r="C239" t="n">
-        <v>0.2965</v>
+        <v>0.5738</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>345</t>
+          <t>341</t>
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.0919</v>
+        <v>0.0683</v>
       </c>
       <c r="C240" t="n">
-        <v>0.1248</v>
+        <v>0.2655</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B241" t="n">
-        <v>-0.008999999999999999</v>
+        <v>0.1499</v>
       </c>
       <c r="C241" t="n">
-        <v>0.0752</v>
+        <v>0.2059</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>347</t>
+          <t>343</t>
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.0297</v>
+        <v>-0.1081</v>
       </c>
       <c r="C242" t="n">
-        <v>0.3054</v>
+        <v>0.2945</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>345</t>
         </is>
       </c>
       <c r="B243" t="n">
-        <v>-0.0256</v>
+        <v>0.06610000000000001</v>
       </c>
       <c r="C243" t="n">
-        <v>0.1678</v>
+        <v>0.1248</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>351</t>
+          <t>346</t>
         </is>
       </c>
       <c r="B244" t="n">
-        <v>0.1212</v>
+        <v>0.0033</v>
       </c>
       <c r="C244" t="n">
-        <v>0.183</v>
+        <v>0.07489999999999999</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>347</t>
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.0518</v>
+        <v>0.0272</v>
       </c>
       <c r="C245" t="n">
-        <v>0.3498</v>
+        <v>0.3053</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>353</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B246" t="n">
-        <v>0.0069</v>
+        <v>0.0113</v>
       </c>
       <c r="C246" t="n">
-        <v>0.4179</v>
+        <v>0.1674</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>354</t>
+          <t>350</t>
         </is>
       </c>
       <c r="B247" t="n">
-        <v>-0.0322</v>
+        <v>0.0784</v>
       </c>
       <c r="C247" t="n">
-        <v>0.1045</v>
+        <v>1.0229</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>359</t>
+          <t>351</t>
         </is>
       </c>
       <c r="B248" t="n">
-        <v>-0.0239</v>
+        <v>-0.07729999999999999</v>
       </c>
       <c r="C248" t="n">
-        <v>0.2192</v>
+        <v>0.1863</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>352</t>
         </is>
       </c>
       <c r="B249" t="n">
-        <v>-0.02</v>
+        <v>0.0225</v>
       </c>
       <c r="C249" t="n">
-        <v>0.2992</v>
+        <v>0.3503</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>353</t>
         </is>
       </c>
       <c r="B250" t="n">
-        <v>0.0058</v>
+        <v>0.015</v>
       </c>
       <c r="C250" t="n">
-        <v>0.5266</v>
+        <v>0.4178</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>362</t>
+          <t>354</t>
         </is>
       </c>
       <c r="B251" t="n">
-        <v>-0.1416</v>
+        <v>-0.0261</v>
       </c>
       <c r="C251" t="n">
-        <v>0.3603</v>
+        <v>0.1043</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>364</t>
+          <t>359</t>
         </is>
       </c>
       <c r="B252" t="n">
-        <v>-0.0004</v>
+        <v>-0.0391</v>
       </c>
       <c r="C252" t="n">
-        <v>0.0891</v>
+        <v>0.2199</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>367</t>
+          <t>360</t>
         </is>
       </c>
       <c r="B253" t="n">
-        <v>-0.0019</v>
+        <v>-0.0278</v>
       </c>
       <c r="C253" t="n">
-        <v>0.2152</v>
+        <v>0.2993</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>369</t>
+          <t>361</t>
         </is>
       </c>
       <c r="B254" t="n">
-        <v>-0.0068</v>
+        <v>0.0075</v>
       </c>
       <c r="C254" t="n">
-        <v>0.1354</v>
+        <v>0.5265</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>370</t>
+          <t>362</t>
         </is>
       </c>
       <c r="B255" t="n">
-        <v>0.0002</v>
+        <v>-0.1006</v>
       </c>
       <c r="C255" t="n">
-        <v>0.1563</v>
+        <v>0.3601</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>372</t>
+          <t>364</t>
         </is>
       </c>
       <c r="B256" t="n">
-        <v>0.0653</v>
+        <v>0.0025</v>
       </c>
       <c r="C256" t="n">
-        <v>0.1791</v>
+        <v>0.0891</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>367</t>
         </is>
       </c>
       <c r="B257" t="n">
-        <v>-0.0119</v>
+        <v>0.0314</v>
       </c>
       <c r="C257" t="n">
-        <v>0.2386</v>
+        <v>0.2153</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>374</t>
+          <t>369</t>
         </is>
       </c>
       <c r="B258" t="n">
-        <v>0.037</v>
+        <v>-0.0172</v>
       </c>
       <c r="C258" t="n">
-        <v>0.2077</v>
+        <v>0.1354</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>376</t>
+          <t>370</t>
         </is>
       </c>
       <c r="B259" t="n">
-        <v>0.0257</v>
+        <v>0.0074</v>
       </c>
       <c r="C259" t="n">
-        <v>0.1905</v>
+        <v>0.1563</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>377</t>
+          <t>372</t>
         </is>
       </c>
       <c r="B260" t="n">
-        <v>0.0098</v>
+        <v>0.0493</v>
       </c>
       <c r="C260" t="n">
-        <v>0.3257</v>
+        <v>0.1794</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>378</t>
+          <t>373</t>
         </is>
       </c>
       <c r="B261" t="n">
-        <v>0.0023</v>
+        <v>-0.0247</v>
       </c>
       <c r="C261" t="n">
-        <v>0.3389</v>
+        <v>0.2385</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>374</t>
         </is>
       </c>
       <c r="B262" t="n">
-        <v>0.0404</v>
+        <v>0.0267</v>
       </c>
       <c r="C262" t="n">
-        <v>0.1054</v>
+        <v>0.2079</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>380</t>
+          <t>376</t>
         </is>
       </c>
       <c r="B263" t="n">
-        <v>0.0209</v>
+        <v>0.0193</v>
       </c>
       <c r="C263" t="n">
-        <v>0.3829</v>
+        <v>0.1905</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>381</t>
+          <t>377</t>
         </is>
       </c>
       <c r="B264" t="n">
-        <v>0.0737</v>
+        <v>-0.0012</v>
       </c>
       <c r="C264" t="n">
-        <v>0.17</v>
+        <v>0.3258</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>382</t>
+          <t>378</t>
         </is>
       </c>
       <c r="B265" t="n">
-        <v>0.0605</v>
+        <v>0.0056</v>
       </c>
       <c r="C265" t="n">
-        <v>0.1581</v>
+        <v>0.3388</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>383</t>
+          <t>379</t>
         </is>
       </c>
       <c r="B266" t="n">
-        <v>-0.0649</v>
+        <v>0.0233</v>
       </c>
       <c r="C266" t="n">
-        <v>0.1884</v>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>385</t>
+          <t>380</t>
         </is>
       </c>
       <c r="B267" t="n">
-        <v>-0.0196</v>
+        <v>0.0147</v>
       </c>
       <c r="C267" t="n">
-        <v>0.0509</v>
+        <v>0.383</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>386</t>
+          <t>381</t>
         </is>
       </c>
       <c r="B268" t="n">
-        <v>-0.0055</v>
+        <v>0.0616</v>
       </c>
       <c r="C268" t="n">
-        <v>0.1014</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>387</t>
+          <t>382</t>
         </is>
       </c>
       <c r="B269" t="n">
-        <v>0.0239</v>
+        <v>0.0541</v>
       </c>
       <c r="C269" t="n">
-        <v>0.1708</v>
+        <v>0.1579</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>388</t>
+          <t>383</t>
         </is>
       </c>
       <c r="B270" t="n">
-        <v>0.0418</v>
+        <v>-0.0857</v>
       </c>
       <c r="C270" t="n">
-        <v>0.2056</v>
+        <v>0.1893</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>389</t>
+          <t>385</t>
         </is>
       </c>
       <c r="B271" t="n">
-        <v>0.003</v>
+        <v>0.0042</v>
       </c>
       <c r="C271" t="n">
-        <v>0.433</v>
+        <v>0.0506</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>386</t>
         </is>
       </c>
       <c r="B272" t="n">
-        <v>0.0272</v>
+        <v>-0.0032</v>
       </c>
       <c r="C272" t="n">
-        <v>0.1196</v>
+        <v>0.1014</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>391</t>
+          <t>387</t>
         </is>
       </c>
       <c r="B273" t="n">
-        <v>0.009299999999999999</v>
+        <v>0.0336</v>
       </c>
       <c r="C273" t="n">
-        <v>0.1519</v>
+        <v>0.1707</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>392</t>
+          <t>388</t>
         </is>
       </c>
       <c r="B274" t="n">
-        <v>0.0036</v>
+        <v>0.0418</v>
       </c>
       <c r="C274" t="n">
-        <v>0.2025</v>
+        <v>0.2056</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>393</t>
+          <t>389</t>
         </is>
       </c>
       <c r="B275" t="n">
-        <v>0.0956</v>
+        <v>0.0008</v>
       </c>
       <c r="C275" t="n">
-        <v>0.3232</v>
+        <v>0.4331</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>394</t>
+          <t>390</t>
         </is>
       </c>
       <c r="B276" t="n">
-        <v>0.0989</v>
+        <v>0.0285</v>
       </c>
       <c r="C276" t="n">
-        <v>0.1515</v>
+        <v>0.1196</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>395</t>
+          <t>391</t>
         </is>
       </c>
       <c r="B277" t="n">
-        <v>0.0046</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="C277" t="n">
-        <v>0.1715</v>
+        <v>0.1519</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>396</t>
+          <t>392</t>
         </is>
       </c>
       <c r="B278" t="n">
-        <v>-0.0136</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="C278" t="n">
-        <v>0.0814</v>
+        <v>0.2025</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>398</t>
+          <t>393</t>
         </is>
       </c>
       <c r="B279" t="n">
-        <v>-0.0123</v>
+        <v>0.0956</v>
       </c>
       <c r="C279" t="n">
-        <v>0.1297</v>
+        <v>0.3232</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>399</t>
+          <t>394</t>
         </is>
       </c>
       <c r="B280" t="n">
-        <v>0.0504</v>
+        <v>0.09619999999999999</v>
       </c>
       <c r="C280" t="n">
-        <v>0.3509</v>
+        <v>0.1516</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
+          <t>395</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>0.0042</v>
+      </c>
+      <c r="C281" t="n">
+        <v>0.1715</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>396</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>-0.0216</v>
+      </c>
+      <c r="C282" t="n">
+        <v>0.0815</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>398</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>-0.0054</v>
+      </c>
+      <c r="C283" t="n">
+        <v>0.1296</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>399</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>0.0486</v>
+      </c>
+      <c r="C284" t="n">
+        <v>0.351</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
           <t>400</t>
         </is>
       </c>
-      <c r="B281" t="n">
-        <v>0.0133</v>
-      </c>
-      <c r="C281" t="n">
+      <c r="B285" t="n">
+        <v>0.0138</v>
+      </c>
+      <c r="C285" t="n">
         <v>0.1265</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add drug's number 384
</commit_message>
<xml_diff>
--- a/deming.xlsx
+++ b/deming.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C285"/>
+  <dimension ref="A1:C286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4142,6 +4142,19 @@
         <v>0.1265</v>
       </c>
     </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>384</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>0.0019</v>
+      </c>
+      <c r="C286" t="n">
+        <v>0.122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>